<commit_message>
Deprecated Finnish Participant Schemes; TICC-345
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.9.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAE61C1-CE7E-42E3-BA75-EF4A1223CCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DE9F89-9BF6-499D-9645-3AC4D6205FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="566">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1985,6 +1985,9 @@
   </si>
   <si>
     <t>The Danish Business Authority - SE-number (DK:SE)</t>
+  </si>
+  <si>
+    <t>8.9</t>
   </si>
 </sst>
 </file>
@@ -2081,7 +2084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2142,6 +2145,9 @@
     </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2774,10 +2780,10 @@
   <dimension ref="A1:AMN102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2800,7 +2806,7 @@
     <col min="16" max="1027" width="14.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1027" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -2888,7 +2894,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -2964,48 +2970,1066 @@
         <v>530</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:1027" s="20" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="G5" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>565</v>
+      </c>
+      <c r="I5" s="18">
+        <v>45657</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="15" t="s">
         <v>396</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="17" t="s">
         <v>530</v>
       </c>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
+      <c r="AO5" s="15"/>
+      <c r="AP5" s="15"/>
+      <c r="AQ5" s="15"/>
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="15"/>
+      <c r="AT5" s="15"/>
+      <c r="AU5" s="15"/>
+      <c r="AV5" s="15"/>
+      <c r="AW5" s="15"/>
+      <c r="AX5" s="15"/>
+      <c r="AY5" s="15"/>
+      <c r="AZ5" s="15"/>
+      <c r="BA5" s="15"/>
+      <c r="BB5" s="15"/>
+      <c r="BC5" s="15"/>
+      <c r="BD5" s="15"/>
+      <c r="BE5" s="15"/>
+      <c r="BF5" s="15"/>
+      <c r="BG5" s="15"/>
+      <c r="BH5" s="15"/>
+      <c r="BI5" s="15"/>
+      <c r="BJ5" s="15"/>
+      <c r="BK5" s="15"/>
+      <c r="BL5" s="15"/>
+      <c r="BM5" s="15"/>
+      <c r="BN5" s="15"/>
+      <c r="BO5" s="15"/>
+      <c r="BP5" s="15"/>
+      <c r="BQ5" s="15"/>
+      <c r="BR5" s="15"/>
+      <c r="BS5" s="15"/>
+      <c r="BT5" s="15"/>
+      <c r="BU5" s="15"/>
+      <c r="BV5" s="15"/>
+      <c r="BW5" s="15"/>
+      <c r="BX5" s="15"/>
+      <c r="BY5" s="15"/>
+      <c r="BZ5" s="15"/>
+      <c r="CA5" s="15"/>
+      <c r="CB5" s="15"/>
+      <c r="CC5" s="15"/>
+      <c r="CD5" s="15"/>
+      <c r="CE5" s="15"/>
+      <c r="CF5" s="15"/>
+      <c r="CG5" s="15"/>
+      <c r="CH5" s="15"/>
+      <c r="CI5" s="15"/>
+      <c r="CJ5" s="15"/>
+      <c r="CK5" s="15"/>
+      <c r="CL5" s="15"/>
+      <c r="CM5" s="15"/>
+      <c r="CN5" s="15"/>
+      <c r="CO5" s="15"/>
+      <c r="CP5" s="15"/>
+      <c r="CQ5" s="15"/>
+      <c r="CR5" s="15"/>
+      <c r="CS5" s="15"/>
+      <c r="CT5" s="15"/>
+      <c r="CU5" s="15"/>
+      <c r="CV5" s="15"/>
+      <c r="CW5" s="15"/>
+      <c r="CX5" s="15"/>
+      <c r="CY5" s="15"/>
+      <c r="CZ5" s="15"/>
+      <c r="DA5" s="15"/>
+      <c r="DB5" s="15"/>
+      <c r="DC5" s="15"/>
+      <c r="DD5" s="15"/>
+      <c r="DE5" s="15"/>
+      <c r="DF5" s="15"/>
+      <c r="DG5" s="15"/>
+      <c r="DH5" s="15"/>
+      <c r="DI5" s="15"/>
+      <c r="DJ5" s="15"/>
+      <c r="DK5" s="15"/>
+      <c r="DL5" s="15"/>
+      <c r="DM5" s="15"/>
+      <c r="DN5" s="15"/>
+      <c r="DO5" s="15"/>
+      <c r="DP5" s="15"/>
+      <c r="DQ5" s="15"/>
+      <c r="DR5" s="15"/>
+      <c r="DS5" s="15"/>
+      <c r="DT5" s="15"/>
+      <c r="DU5" s="15"/>
+      <c r="DV5" s="15"/>
+      <c r="DW5" s="15"/>
+      <c r="DX5" s="15"/>
+      <c r="DY5" s="15"/>
+      <c r="DZ5" s="15"/>
+      <c r="EA5" s="15"/>
+      <c r="EB5" s="15"/>
+      <c r="EC5" s="15"/>
+      <c r="ED5" s="15"/>
+      <c r="EE5" s="15"/>
+      <c r="EF5" s="15"/>
+      <c r="EG5" s="15"/>
+      <c r="EH5" s="15"/>
+      <c r="EI5" s="15"/>
+      <c r="EJ5" s="15"/>
+      <c r="EK5" s="15"/>
+      <c r="EL5" s="15"/>
+      <c r="EM5" s="15"/>
+      <c r="EN5" s="15"/>
+      <c r="EO5" s="15"/>
+      <c r="EP5" s="15"/>
+      <c r="EQ5" s="15"/>
+      <c r="ER5" s="15"/>
+      <c r="ES5" s="15"/>
+      <c r="ET5" s="15"/>
+      <c r="EU5" s="15"/>
+      <c r="EV5" s="15"/>
+      <c r="EW5" s="15"/>
+      <c r="EX5" s="15"/>
+      <c r="EY5" s="15"/>
+      <c r="EZ5" s="15"/>
+      <c r="FA5" s="15"/>
+      <c r="FB5" s="15"/>
+      <c r="FC5" s="15"/>
+      <c r="FD5" s="15"/>
+      <c r="FE5" s="15"/>
+      <c r="FF5" s="15"/>
+      <c r="FG5" s="15"/>
+      <c r="FH5" s="15"/>
+      <c r="FI5" s="15"/>
+      <c r="FJ5" s="15"/>
+      <c r="FK5" s="15"/>
+      <c r="FL5" s="15"/>
+      <c r="FM5" s="15"/>
+      <c r="FN5" s="15"/>
+      <c r="FO5" s="15"/>
+      <c r="FP5" s="15"/>
+      <c r="FQ5" s="15"/>
+      <c r="FR5" s="15"/>
+      <c r="FS5" s="15"/>
+      <c r="FT5" s="15"/>
+      <c r="FU5" s="15"/>
+      <c r="FV5" s="15"/>
+      <c r="FW5" s="15"/>
+      <c r="FX5" s="15"/>
+      <c r="FY5" s="15"/>
+      <c r="FZ5" s="15"/>
+      <c r="GA5" s="15"/>
+      <c r="GB5" s="15"/>
+      <c r="GC5" s="15"/>
+      <c r="GD5" s="15"/>
+      <c r="GE5" s="15"/>
+      <c r="GF5" s="15"/>
+      <c r="GG5" s="15"/>
+      <c r="GH5" s="15"/>
+      <c r="GI5" s="15"/>
+      <c r="GJ5" s="15"/>
+      <c r="GK5" s="15"/>
+      <c r="GL5" s="15"/>
+      <c r="GM5" s="15"/>
+      <c r="GN5" s="15"/>
+      <c r="GO5" s="15"/>
+      <c r="GP5" s="15"/>
+      <c r="GQ5" s="15"/>
+      <c r="GR5" s="15"/>
+      <c r="GS5" s="15"/>
+      <c r="GT5" s="15"/>
+      <c r="GU5" s="15"/>
+      <c r="GV5" s="15"/>
+      <c r="GW5" s="15"/>
+      <c r="GX5" s="15"/>
+      <c r="GY5" s="15"/>
+      <c r="GZ5" s="15"/>
+      <c r="HA5" s="15"/>
+      <c r="HB5" s="15"/>
+      <c r="HC5" s="15"/>
+      <c r="HD5" s="15"/>
+      <c r="HE5" s="15"/>
+      <c r="HF5" s="15"/>
+      <c r="HG5" s="15"/>
+      <c r="HH5" s="15"/>
+      <c r="HI5" s="15"/>
+      <c r="HJ5" s="15"/>
+      <c r="HK5" s="15"/>
+      <c r="HL5" s="15"/>
+      <c r="HM5" s="15"/>
+      <c r="HN5" s="15"/>
+      <c r="HO5" s="15"/>
+      <c r="HP5" s="15"/>
+      <c r="HQ5" s="15"/>
+      <c r="HR5" s="15"/>
+      <c r="HS5" s="15"/>
+      <c r="HT5" s="15"/>
+      <c r="HU5" s="15"/>
+      <c r="HV5" s="15"/>
+      <c r="HW5" s="15"/>
+      <c r="HX5" s="15"/>
+      <c r="HY5" s="15"/>
+      <c r="HZ5" s="15"/>
+      <c r="IA5" s="15"/>
+      <c r="IB5" s="15"/>
+      <c r="IC5" s="15"/>
+      <c r="ID5" s="15"/>
+      <c r="IE5" s="15"/>
+      <c r="IF5" s="15"/>
+      <c r="IG5" s="15"/>
+      <c r="IH5" s="15"/>
+      <c r="II5" s="15"/>
+      <c r="IJ5" s="15"/>
+      <c r="IK5" s="15"/>
+      <c r="IL5" s="15"/>
+      <c r="IM5" s="15"/>
+      <c r="IN5" s="15"/>
+      <c r="IO5" s="15"/>
+      <c r="IP5" s="15"/>
+      <c r="IQ5" s="15"/>
+      <c r="IR5" s="15"/>
+      <c r="IS5" s="15"/>
+      <c r="IT5" s="15"/>
+      <c r="IU5" s="15"/>
+      <c r="IV5" s="15"/>
+      <c r="IW5" s="15"/>
+      <c r="IX5" s="15"/>
+      <c r="IY5" s="15"/>
+      <c r="IZ5" s="15"/>
+      <c r="JA5" s="15"/>
+      <c r="JB5" s="15"/>
+      <c r="JC5" s="15"/>
+      <c r="JD5" s="15"/>
+      <c r="JE5" s="15"/>
+      <c r="JF5" s="15"/>
+      <c r="JG5" s="15"/>
+      <c r="JH5" s="15"/>
+      <c r="JI5" s="15"/>
+      <c r="JJ5" s="15"/>
+      <c r="JK5" s="15"/>
+      <c r="JL5" s="15"/>
+      <c r="JM5" s="15"/>
+      <c r="JN5" s="15"/>
+      <c r="JO5" s="15"/>
+      <c r="JP5" s="15"/>
+      <c r="JQ5" s="15"/>
+      <c r="JR5" s="15"/>
+      <c r="JS5" s="15"/>
+      <c r="JT5" s="15"/>
+      <c r="JU5" s="15"/>
+      <c r="JV5" s="15"/>
+      <c r="JW5" s="15"/>
+      <c r="JX5" s="15"/>
+      <c r="JY5" s="15"/>
+      <c r="JZ5" s="15"/>
+      <c r="KA5" s="15"/>
+      <c r="KB5" s="15"/>
+      <c r="KC5" s="15"/>
+      <c r="KD5" s="15"/>
+      <c r="KE5" s="15"/>
+      <c r="KF5" s="15"/>
+      <c r="KG5" s="15"/>
+      <c r="KH5" s="15"/>
+      <c r="KI5" s="15"/>
+      <c r="KJ5" s="15"/>
+      <c r="KK5" s="15"/>
+      <c r="KL5" s="15"/>
+      <c r="KM5" s="15"/>
+      <c r="KN5" s="15"/>
+      <c r="KO5" s="15"/>
+      <c r="KP5" s="15"/>
+      <c r="KQ5" s="15"/>
+      <c r="KR5" s="15"/>
+      <c r="KS5" s="15"/>
+      <c r="KT5" s="15"/>
+      <c r="KU5" s="15"/>
+      <c r="KV5" s="15"/>
+      <c r="KW5" s="15"/>
+      <c r="KX5" s="15"/>
+      <c r="KY5" s="15"/>
+      <c r="KZ5" s="15"/>
+      <c r="LA5" s="15"/>
+      <c r="LB5" s="15"/>
+      <c r="LC5" s="15"/>
+      <c r="LD5" s="15"/>
+      <c r="LE5" s="15"/>
+      <c r="LF5" s="15"/>
+      <c r="LG5" s="15"/>
+      <c r="LH5" s="15"/>
+      <c r="LI5" s="15"/>
+      <c r="LJ5" s="15"/>
+      <c r="LK5" s="15"/>
+      <c r="LL5" s="15"/>
+      <c r="LM5" s="15"/>
+      <c r="LN5" s="15"/>
+      <c r="LO5" s="15"/>
+      <c r="LP5" s="15"/>
+      <c r="LQ5" s="15"/>
+      <c r="LR5" s="15"/>
+      <c r="LS5" s="15"/>
+      <c r="LT5" s="15"/>
+      <c r="LU5" s="15"/>
+      <c r="LV5" s="15"/>
+      <c r="LW5" s="15"/>
+      <c r="LX5" s="15"/>
+      <c r="LY5" s="15"/>
+      <c r="LZ5" s="15"/>
+      <c r="MA5" s="15"/>
+      <c r="MB5" s="15"/>
+      <c r="MC5" s="15"/>
+      <c r="MD5" s="15"/>
+      <c r="ME5" s="15"/>
+      <c r="MF5" s="15"/>
+      <c r="MG5" s="15"/>
+      <c r="MH5" s="15"/>
+      <c r="MI5" s="15"/>
+      <c r="MJ5" s="15"/>
+      <c r="MK5" s="15"/>
+      <c r="ML5" s="15"/>
+      <c r="MM5" s="15"/>
+      <c r="MN5" s="15"/>
+      <c r="MO5" s="15"/>
+      <c r="MP5" s="15"/>
+      <c r="MQ5" s="15"/>
+      <c r="MR5" s="15"/>
+      <c r="MS5" s="15"/>
+      <c r="MT5" s="15"/>
+      <c r="MU5" s="15"/>
+      <c r="MV5" s="15"/>
+      <c r="MW5" s="15"/>
+      <c r="MX5" s="15"/>
+      <c r="MY5" s="15"/>
+      <c r="MZ5" s="15"/>
+      <c r="NA5" s="15"/>
+      <c r="NB5" s="15"/>
+      <c r="NC5" s="15"/>
+      <c r="ND5" s="15"/>
+      <c r="NE5" s="15"/>
+      <c r="NF5" s="15"/>
+      <c r="NG5" s="15"/>
+      <c r="NH5" s="15"/>
+      <c r="NI5" s="15"/>
+      <c r="NJ5" s="15"/>
+      <c r="NK5" s="15"/>
+      <c r="NL5" s="15"/>
+      <c r="NM5" s="15"/>
+      <c r="NN5" s="15"/>
+      <c r="NO5" s="15"/>
+      <c r="NP5" s="15"/>
+      <c r="NQ5" s="15"/>
+      <c r="NR5" s="15"/>
+      <c r="NS5" s="15"/>
+      <c r="NT5" s="15"/>
+      <c r="NU5" s="15"/>
+      <c r="NV5" s="15"/>
+      <c r="NW5" s="15"/>
+      <c r="NX5" s="15"/>
+      <c r="NY5" s="15"/>
+      <c r="NZ5" s="15"/>
+      <c r="OA5" s="15"/>
+      <c r="OB5" s="15"/>
+      <c r="OC5" s="15"/>
+      <c r="OD5" s="15"/>
+      <c r="OE5" s="15"/>
+      <c r="OF5" s="15"/>
+      <c r="OG5" s="15"/>
+      <c r="OH5" s="15"/>
+      <c r="OI5" s="15"/>
+      <c r="OJ5" s="15"/>
+      <c r="OK5" s="15"/>
+      <c r="OL5" s="15"/>
+      <c r="OM5" s="15"/>
+      <c r="ON5" s="15"/>
+      <c r="OO5" s="15"/>
+      <c r="OP5" s="15"/>
+      <c r="OQ5" s="15"/>
+      <c r="OR5" s="15"/>
+      <c r="OS5" s="15"/>
+      <c r="OT5" s="15"/>
+      <c r="OU5" s="15"/>
+      <c r="OV5" s="15"/>
+      <c r="OW5" s="15"/>
+      <c r="OX5" s="15"/>
+      <c r="OY5" s="15"/>
+      <c r="OZ5" s="15"/>
+      <c r="PA5" s="15"/>
+      <c r="PB5" s="15"/>
+      <c r="PC5" s="15"/>
+      <c r="PD5" s="15"/>
+      <c r="PE5" s="15"/>
+      <c r="PF5" s="15"/>
+      <c r="PG5" s="15"/>
+      <c r="PH5" s="15"/>
+      <c r="PI5" s="15"/>
+      <c r="PJ5" s="15"/>
+      <c r="PK5" s="15"/>
+      <c r="PL5" s="15"/>
+      <c r="PM5" s="15"/>
+      <c r="PN5" s="15"/>
+      <c r="PO5" s="15"/>
+      <c r="PP5" s="15"/>
+      <c r="PQ5" s="15"/>
+      <c r="PR5" s="15"/>
+      <c r="PS5" s="15"/>
+      <c r="PT5" s="15"/>
+      <c r="PU5" s="15"/>
+      <c r="PV5" s="15"/>
+      <c r="PW5" s="15"/>
+      <c r="PX5" s="15"/>
+      <c r="PY5" s="15"/>
+      <c r="PZ5" s="15"/>
+      <c r="QA5" s="15"/>
+      <c r="QB5" s="15"/>
+      <c r="QC5" s="15"/>
+      <c r="QD5" s="15"/>
+      <c r="QE5" s="15"/>
+      <c r="QF5" s="15"/>
+      <c r="QG5" s="15"/>
+      <c r="QH5" s="15"/>
+      <c r="QI5" s="15"/>
+      <c r="QJ5" s="15"/>
+      <c r="QK5" s="15"/>
+      <c r="QL5" s="15"/>
+      <c r="QM5" s="15"/>
+      <c r="QN5" s="15"/>
+      <c r="QO5" s="15"/>
+      <c r="QP5" s="15"/>
+      <c r="QQ5" s="15"/>
+      <c r="QR5" s="15"/>
+      <c r="QS5" s="15"/>
+      <c r="QT5" s="15"/>
+      <c r="QU5" s="15"/>
+      <c r="QV5" s="15"/>
+      <c r="QW5" s="15"/>
+      <c r="QX5" s="15"/>
+      <c r="QY5" s="15"/>
+      <c r="QZ5" s="15"/>
+      <c r="RA5" s="15"/>
+      <c r="RB5" s="15"/>
+      <c r="RC5" s="15"/>
+      <c r="RD5" s="15"/>
+      <c r="RE5" s="15"/>
+      <c r="RF5" s="15"/>
+      <c r="RG5" s="15"/>
+      <c r="RH5" s="15"/>
+      <c r="RI5" s="15"/>
+      <c r="RJ5" s="15"/>
+      <c r="RK5" s="15"/>
+      <c r="RL5" s="15"/>
+      <c r="RM5" s="15"/>
+      <c r="RN5" s="15"/>
+      <c r="RO5" s="15"/>
+      <c r="RP5" s="15"/>
+      <c r="RQ5" s="15"/>
+      <c r="RR5" s="15"/>
+      <c r="RS5" s="15"/>
+      <c r="RT5" s="15"/>
+      <c r="RU5" s="15"/>
+      <c r="RV5" s="15"/>
+      <c r="RW5" s="15"/>
+      <c r="RX5" s="15"/>
+      <c r="RY5" s="15"/>
+      <c r="RZ5" s="15"/>
+      <c r="SA5" s="15"/>
+      <c r="SB5" s="15"/>
+      <c r="SC5" s="15"/>
+      <c r="SD5" s="15"/>
+      <c r="SE5" s="15"/>
+      <c r="SF5" s="15"/>
+      <c r="SG5" s="15"/>
+      <c r="SH5" s="15"/>
+      <c r="SI5" s="15"/>
+      <c r="SJ5" s="15"/>
+      <c r="SK5" s="15"/>
+      <c r="SL5" s="15"/>
+      <c r="SM5" s="15"/>
+      <c r="SN5" s="15"/>
+      <c r="SO5" s="15"/>
+      <c r="SP5" s="15"/>
+      <c r="SQ5" s="15"/>
+      <c r="SR5" s="15"/>
+      <c r="SS5" s="15"/>
+      <c r="ST5" s="15"/>
+      <c r="SU5" s="15"/>
+      <c r="SV5" s="15"/>
+      <c r="SW5" s="15"/>
+      <c r="SX5" s="15"/>
+      <c r="SY5" s="15"/>
+      <c r="SZ5" s="15"/>
+      <c r="TA5" s="15"/>
+      <c r="TB5" s="15"/>
+      <c r="TC5" s="15"/>
+      <c r="TD5" s="15"/>
+      <c r="TE5" s="15"/>
+      <c r="TF5" s="15"/>
+      <c r="TG5" s="15"/>
+      <c r="TH5" s="15"/>
+      <c r="TI5" s="15"/>
+      <c r="TJ5" s="15"/>
+      <c r="TK5" s="15"/>
+      <c r="TL5" s="15"/>
+      <c r="TM5" s="15"/>
+      <c r="TN5" s="15"/>
+      <c r="TO5" s="15"/>
+      <c r="TP5" s="15"/>
+      <c r="TQ5" s="15"/>
+      <c r="TR5" s="15"/>
+      <c r="TS5" s="15"/>
+      <c r="TT5" s="15"/>
+      <c r="TU5" s="15"/>
+      <c r="TV5" s="15"/>
+      <c r="TW5" s="15"/>
+      <c r="TX5" s="15"/>
+      <c r="TY5" s="15"/>
+      <c r="TZ5" s="15"/>
+      <c r="UA5" s="15"/>
+      <c r="UB5" s="15"/>
+      <c r="UC5" s="15"/>
+      <c r="UD5" s="15"/>
+      <c r="UE5" s="15"/>
+      <c r="UF5" s="15"/>
+      <c r="UG5" s="15"/>
+      <c r="UH5" s="15"/>
+      <c r="UI5" s="15"/>
+      <c r="UJ5" s="15"/>
+      <c r="UK5" s="15"/>
+      <c r="UL5" s="15"/>
+      <c r="UM5" s="15"/>
+      <c r="UN5" s="15"/>
+      <c r="UO5" s="15"/>
+      <c r="UP5" s="15"/>
+      <c r="UQ5" s="15"/>
+      <c r="UR5" s="15"/>
+      <c r="US5" s="15"/>
+      <c r="UT5" s="15"/>
+      <c r="UU5" s="15"/>
+      <c r="UV5" s="15"/>
+      <c r="UW5" s="15"/>
+      <c r="UX5" s="15"/>
+      <c r="UY5" s="15"/>
+      <c r="UZ5" s="15"/>
+      <c r="VA5" s="15"/>
+      <c r="VB5" s="15"/>
+      <c r="VC5" s="15"/>
+      <c r="VD5" s="15"/>
+      <c r="VE5" s="15"/>
+      <c r="VF5" s="15"/>
+      <c r="VG5" s="15"/>
+      <c r="VH5" s="15"/>
+      <c r="VI5" s="15"/>
+      <c r="VJ5" s="15"/>
+      <c r="VK5" s="15"/>
+      <c r="VL5" s="15"/>
+      <c r="VM5" s="15"/>
+      <c r="VN5" s="15"/>
+      <c r="VO5" s="15"/>
+      <c r="VP5" s="15"/>
+      <c r="VQ5" s="15"/>
+      <c r="VR5" s="15"/>
+      <c r="VS5" s="15"/>
+      <c r="VT5" s="15"/>
+      <c r="VU5" s="15"/>
+      <c r="VV5" s="15"/>
+      <c r="VW5" s="15"/>
+      <c r="VX5" s="15"/>
+      <c r="VY5" s="15"/>
+      <c r="VZ5" s="15"/>
+      <c r="WA5" s="15"/>
+      <c r="WB5" s="15"/>
+      <c r="WC5" s="15"/>
+      <c r="WD5" s="15"/>
+      <c r="WE5" s="15"/>
+      <c r="WF5" s="15"/>
+      <c r="WG5" s="15"/>
+      <c r="WH5" s="15"/>
+      <c r="WI5" s="15"/>
+      <c r="WJ5" s="15"/>
+      <c r="WK5" s="15"/>
+      <c r="WL5" s="15"/>
+      <c r="WM5" s="15"/>
+      <c r="WN5" s="15"/>
+      <c r="WO5" s="15"/>
+      <c r="WP5" s="15"/>
+      <c r="WQ5" s="15"/>
+      <c r="WR5" s="15"/>
+      <c r="WS5" s="15"/>
+      <c r="WT5" s="15"/>
+      <c r="WU5" s="15"/>
+      <c r="WV5" s="15"/>
+      <c r="WW5" s="15"/>
+      <c r="WX5" s="15"/>
+      <c r="WY5" s="15"/>
+      <c r="WZ5" s="15"/>
+      <c r="XA5" s="15"/>
+      <c r="XB5" s="15"/>
+      <c r="XC5" s="15"/>
+      <c r="XD5" s="15"/>
+      <c r="XE5" s="15"/>
+      <c r="XF5" s="15"/>
+      <c r="XG5" s="15"/>
+      <c r="XH5" s="15"/>
+      <c r="XI5" s="15"/>
+      <c r="XJ5" s="15"/>
+      <c r="XK5" s="15"/>
+      <c r="XL5" s="15"/>
+      <c r="XM5" s="15"/>
+      <c r="XN5" s="15"/>
+      <c r="XO5" s="15"/>
+      <c r="XP5" s="15"/>
+      <c r="XQ5" s="15"/>
+      <c r="XR5" s="15"/>
+      <c r="XS5" s="15"/>
+      <c r="XT5" s="15"/>
+      <c r="XU5" s="15"/>
+      <c r="XV5" s="15"/>
+      <c r="XW5" s="15"/>
+      <c r="XX5" s="15"/>
+      <c r="XY5" s="15"/>
+      <c r="XZ5" s="15"/>
+      <c r="YA5" s="15"/>
+      <c r="YB5" s="15"/>
+      <c r="YC5" s="15"/>
+      <c r="YD5" s="15"/>
+      <c r="YE5" s="15"/>
+      <c r="YF5" s="15"/>
+      <c r="YG5" s="15"/>
+      <c r="YH5" s="15"/>
+      <c r="YI5" s="15"/>
+      <c r="YJ5" s="15"/>
+      <c r="YK5" s="15"/>
+      <c r="YL5" s="15"/>
+      <c r="YM5" s="15"/>
+      <c r="YN5" s="15"/>
+      <c r="YO5" s="15"/>
+      <c r="YP5" s="15"/>
+      <c r="YQ5" s="15"/>
+      <c r="YR5" s="15"/>
+      <c r="YS5" s="15"/>
+      <c r="YT5" s="15"/>
+      <c r="YU5" s="15"/>
+      <c r="YV5" s="15"/>
+      <c r="YW5" s="15"/>
+      <c r="YX5" s="15"/>
+      <c r="YY5" s="15"/>
+      <c r="YZ5" s="15"/>
+      <c r="ZA5" s="15"/>
+      <c r="ZB5" s="15"/>
+      <c r="ZC5" s="15"/>
+      <c r="ZD5" s="15"/>
+      <c r="ZE5" s="15"/>
+      <c r="ZF5" s="15"/>
+      <c r="ZG5" s="15"/>
+      <c r="ZH5" s="15"/>
+      <c r="ZI5" s="15"/>
+      <c r="ZJ5" s="15"/>
+      <c r="ZK5" s="15"/>
+      <c r="ZL5" s="15"/>
+      <c r="ZM5" s="15"/>
+      <c r="ZN5" s="15"/>
+      <c r="ZO5" s="15"/>
+      <c r="ZP5" s="15"/>
+      <c r="ZQ5" s="15"/>
+      <c r="ZR5" s="15"/>
+      <c r="ZS5" s="15"/>
+      <c r="ZT5" s="15"/>
+      <c r="ZU5" s="15"/>
+      <c r="ZV5" s="15"/>
+      <c r="ZW5" s="15"/>
+      <c r="ZX5" s="15"/>
+      <c r="ZY5" s="15"/>
+      <c r="ZZ5" s="15"/>
+      <c r="AAA5" s="15"/>
+      <c r="AAB5" s="15"/>
+      <c r="AAC5" s="15"/>
+      <c r="AAD5" s="15"/>
+      <c r="AAE5" s="15"/>
+      <c r="AAF5" s="15"/>
+      <c r="AAG5" s="15"/>
+      <c r="AAH5" s="15"/>
+      <c r="AAI5" s="15"/>
+      <c r="AAJ5" s="15"/>
+      <c r="AAK5" s="15"/>
+      <c r="AAL5" s="15"/>
+      <c r="AAM5" s="15"/>
+      <c r="AAN5" s="15"/>
+      <c r="AAO5" s="15"/>
+      <c r="AAP5" s="15"/>
+      <c r="AAQ5" s="15"/>
+      <c r="AAR5" s="15"/>
+      <c r="AAS5" s="15"/>
+      <c r="AAT5" s="15"/>
+      <c r="AAU5" s="15"/>
+      <c r="AAV5" s="15"/>
+      <c r="AAW5" s="15"/>
+      <c r="AAX5" s="15"/>
+      <c r="AAY5" s="15"/>
+      <c r="AAZ5" s="15"/>
+      <c r="ABA5" s="15"/>
+      <c r="ABB5" s="15"/>
+      <c r="ABC5" s="15"/>
+      <c r="ABD5" s="15"/>
+      <c r="ABE5" s="15"/>
+      <c r="ABF5" s="15"/>
+      <c r="ABG5" s="15"/>
+      <c r="ABH5" s="15"/>
+      <c r="ABI5" s="15"/>
+      <c r="ABJ5" s="15"/>
+      <c r="ABK5" s="15"/>
+      <c r="ABL5" s="15"/>
+      <c r="ABM5" s="15"/>
+      <c r="ABN5" s="15"/>
+      <c r="ABO5" s="15"/>
+      <c r="ABP5" s="15"/>
+      <c r="ABQ5" s="15"/>
+      <c r="ABR5" s="15"/>
+      <c r="ABS5" s="15"/>
+      <c r="ABT5" s="15"/>
+      <c r="ABU5" s="15"/>
+      <c r="ABV5" s="15"/>
+      <c r="ABW5" s="15"/>
+      <c r="ABX5" s="15"/>
+      <c r="ABY5" s="15"/>
+      <c r="ABZ5" s="15"/>
+      <c r="ACA5" s="15"/>
+      <c r="ACB5" s="15"/>
+      <c r="ACC5" s="15"/>
+      <c r="ACD5" s="15"/>
+      <c r="ACE5" s="15"/>
+      <c r="ACF5" s="15"/>
+      <c r="ACG5" s="15"/>
+      <c r="ACH5" s="15"/>
+      <c r="ACI5" s="15"/>
+      <c r="ACJ5" s="15"/>
+      <c r="ACK5" s="15"/>
+      <c r="ACL5" s="15"/>
+      <c r="ACM5" s="15"/>
+      <c r="ACN5" s="15"/>
+      <c r="ACO5" s="15"/>
+      <c r="ACP5" s="15"/>
+      <c r="ACQ5" s="15"/>
+      <c r="ACR5" s="15"/>
+      <c r="ACS5" s="15"/>
+      <c r="ACT5" s="15"/>
+      <c r="ACU5" s="15"/>
+      <c r="ACV5" s="15"/>
+      <c r="ACW5" s="15"/>
+      <c r="ACX5" s="15"/>
+      <c r="ACY5" s="15"/>
+      <c r="ACZ5" s="15"/>
+      <c r="ADA5" s="15"/>
+      <c r="ADB5" s="15"/>
+      <c r="ADC5" s="15"/>
+      <c r="ADD5" s="15"/>
+      <c r="ADE5" s="15"/>
+      <c r="ADF5" s="15"/>
+      <c r="ADG5" s="15"/>
+      <c r="ADH5" s="15"/>
+      <c r="ADI5" s="15"/>
+      <c r="ADJ5" s="15"/>
+      <c r="ADK5" s="15"/>
+      <c r="ADL5" s="15"/>
+      <c r="ADM5" s="15"/>
+      <c r="ADN5" s="15"/>
+      <c r="ADO5" s="15"/>
+      <c r="ADP5" s="15"/>
+      <c r="ADQ5" s="15"/>
+      <c r="ADR5" s="15"/>
+      <c r="ADS5" s="15"/>
+      <c r="ADT5" s="15"/>
+      <c r="ADU5" s="15"/>
+      <c r="ADV5" s="15"/>
+      <c r="ADW5" s="15"/>
+      <c r="ADX5" s="15"/>
+      <c r="ADY5" s="15"/>
+      <c r="ADZ5" s="15"/>
+      <c r="AEA5" s="15"/>
+      <c r="AEB5" s="15"/>
+      <c r="AEC5" s="15"/>
+      <c r="AED5" s="15"/>
+      <c r="AEE5" s="15"/>
+      <c r="AEF5" s="15"/>
+      <c r="AEG5" s="15"/>
+      <c r="AEH5" s="15"/>
+      <c r="AEI5" s="15"/>
+      <c r="AEJ5" s="15"/>
+      <c r="AEK5" s="15"/>
+      <c r="AEL5" s="15"/>
+      <c r="AEM5" s="15"/>
+      <c r="AEN5" s="15"/>
+      <c r="AEO5" s="15"/>
+      <c r="AEP5" s="15"/>
+      <c r="AEQ5" s="15"/>
+      <c r="AER5" s="15"/>
+      <c r="AES5" s="15"/>
+      <c r="AET5" s="15"/>
+      <c r="AEU5" s="15"/>
+      <c r="AEV5" s="15"/>
+      <c r="AEW5" s="15"/>
+      <c r="AEX5" s="15"/>
+      <c r="AEY5" s="15"/>
+      <c r="AEZ5" s="15"/>
+      <c r="AFA5" s="15"/>
+      <c r="AFB5" s="15"/>
+      <c r="AFC5" s="15"/>
+      <c r="AFD5" s="15"/>
+      <c r="AFE5" s="15"/>
+      <c r="AFF5" s="15"/>
+      <c r="AFG5" s="15"/>
+      <c r="AFH5" s="15"/>
+      <c r="AFI5" s="15"/>
+      <c r="AFJ5" s="15"/>
+      <c r="AFK5" s="15"/>
+      <c r="AFL5" s="15"/>
+      <c r="AFM5" s="15"/>
+      <c r="AFN5" s="15"/>
+      <c r="AFO5" s="15"/>
+      <c r="AFP5" s="15"/>
+      <c r="AFQ5" s="15"/>
+      <c r="AFR5" s="15"/>
+      <c r="AFS5" s="15"/>
+      <c r="AFT5" s="15"/>
+      <c r="AFU5" s="15"/>
+      <c r="AFV5" s="15"/>
+      <c r="AFW5" s="15"/>
+      <c r="AFX5" s="15"/>
+      <c r="AFY5" s="15"/>
+      <c r="AFZ5" s="15"/>
+      <c r="AGA5" s="15"/>
+      <c r="AGB5" s="15"/>
+      <c r="AGC5" s="15"/>
+      <c r="AGD5" s="15"/>
+      <c r="AGE5" s="15"/>
+      <c r="AGF5" s="15"/>
+      <c r="AGG5" s="15"/>
+      <c r="AGH5" s="15"/>
+      <c r="AGI5" s="15"/>
+      <c r="AGJ5" s="15"/>
+      <c r="AGK5" s="15"/>
+      <c r="AGL5" s="15"/>
+      <c r="AGM5" s="15"/>
+      <c r="AGN5" s="15"/>
+      <c r="AGO5" s="15"/>
+      <c r="AGP5" s="15"/>
+      <c r="AGQ5" s="15"/>
+      <c r="AGR5" s="15"/>
+      <c r="AGS5" s="15"/>
+      <c r="AGT5" s="15"/>
+      <c r="AGU5" s="15"/>
+      <c r="AGV5" s="15"/>
+      <c r="AGW5" s="15"/>
+      <c r="AGX5" s="15"/>
+      <c r="AGY5" s="15"/>
+      <c r="AGZ5" s="15"/>
+      <c r="AHA5" s="15"/>
+      <c r="AHB5" s="15"/>
+      <c r="AHC5" s="15"/>
+      <c r="AHD5" s="15"/>
+      <c r="AHE5" s="15"/>
+      <c r="AHF5" s="15"/>
+      <c r="AHG5" s="15"/>
+      <c r="AHH5" s="15"/>
+      <c r="AHI5" s="15"/>
+      <c r="AHJ5" s="15"/>
+      <c r="AHK5" s="15"/>
+      <c r="AHL5" s="15"/>
+      <c r="AHM5" s="15"/>
+      <c r="AHN5" s="15"/>
+      <c r="AHO5" s="15"/>
+      <c r="AHP5" s="15"/>
+      <c r="AHQ5" s="15"/>
+      <c r="AHR5" s="15"/>
+      <c r="AHS5" s="15"/>
+      <c r="AHT5" s="15"/>
+      <c r="AHU5" s="15"/>
+      <c r="AHV5" s="15"/>
+      <c r="AHW5" s="15"/>
+      <c r="AHX5" s="15"/>
+      <c r="AHY5" s="15"/>
+      <c r="AHZ5" s="15"/>
+      <c r="AIA5" s="15"/>
+      <c r="AIB5" s="15"/>
+      <c r="AIC5" s="15"/>
+      <c r="AID5" s="15"/>
+      <c r="AIE5" s="15"/>
+      <c r="AIF5" s="15"/>
+      <c r="AIG5" s="15"/>
+      <c r="AIH5" s="15"/>
+      <c r="AII5" s="15"/>
+      <c r="AIJ5" s="15"/>
+      <c r="AIK5" s="15"/>
+      <c r="AIL5" s="15"/>
+      <c r="AIM5" s="15"/>
+      <c r="AIN5" s="15"/>
+      <c r="AIO5" s="15"/>
+      <c r="AIP5" s="15"/>
+      <c r="AIQ5" s="15"/>
+      <c r="AIR5" s="15"/>
+      <c r="AIS5" s="15"/>
+      <c r="AIT5" s="15"/>
+      <c r="AIU5" s="15"/>
+      <c r="AIV5" s="15"/>
+      <c r="AIW5" s="15"/>
+      <c r="AIX5" s="15"/>
+      <c r="AIY5" s="15"/>
+      <c r="AIZ5" s="15"/>
+      <c r="AJA5" s="15"/>
+      <c r="AJB5" s="15"/>
+      <c r="AJC5" s="15"/>
+      <c r="AJD5" s="15"/>
+      <c r="AJE5" s="15"/>
+      <c r="AJF5" s="15"/>
+      <c r="AJG5" s="15"/>
+      <c r="AJH5" s="15"/>
+      <c r="AJI5" s="15"/>
+      <c r="AJJ5" s="15"/>
+      <c r="AJK5" s="15"/>
+      <c r="AJL5" s="15"/>
+      <c r="AJM5" s="15"/>
+      <c r="AJN5" s="15"/>
+      <c r="AJO5" s="15"/>
+      <c r="AJP5" s="15"/>
+      <c r="AJQ5" s="15"/>
+      <c r="AJR5" s="15"/>
+      <c r="AJS5" s="15"/>
+      <c r="AJT5" s="15"/>
+      <c r="AJU5" s="15"/>
+      <c r="AJV5" s="15"/>
+      <c r="AJW5" s="15"/>
+      <c r="AJX5" s="15"/>
+      <c r="AJY5" s="15"/>
+      <c r="AJZ5" s="15"/>
+      <c r="AKA5" s="15"/>
+      <c r="AKB5" s="15"/>
+      <c r="AKC5" s="15"/>
+      <c r="AKD5" s="15"/>
+      <c r="AKE5" s="15"/>
+      <c r="AKF5" s="15"/>
+      <c r="AKG5" s="15"/>
+      <c r="AKH5" s="15"/>
+      <c r="AKI5" s="15"/>
+      <c r="AKJ5" s="15"/>
+      <c r="AKK5" s="15"/>
+      <c r="AKL5" s="15"/>
+      <c r="AKM5" s="15"/>
+      <c r="AKN5" s="15"/>
+      <c r="AKO5" s="15"/>
+      <c r="AKP5" s="15"/>
+      <c r="AKQ5" s="15"/>
+      <c r="AKR5" s="15"/>
+      <c r="AKS5" s="15"/>
+      <c r="AKT5" s="15"/>
+      <c r="AKU5" s="15"/>
+      <c r="AKV5" s="15"/>
+      <c r="AKW5" s="15"/>
+      <c r="AKX5" s="15"/>
+      <c r="AKY5" s="15"/>
+      <c r="AKZ5" s="15"/>
+      <c r="ALA5" s="15"/>
+      <c r="ALB5" s="15"/>
+      <c r="ALC5" s="15"/>
+      <c r="ALD5" s="15"/>
+      <c r="ALE5" s="15"/>
+      <c r="ALF5" s="15"/>
+      <c r="ALG5" s="15"/>
+      <c r="ALH5" s="15"/>
+      <c r="ALI5" s="15"/>
+      <c r="ALJ5" s="15"/>
+      <c r="ALK5" s="15"/>
+      <c r="ALL5" s="15"/>
+      <c r="ALM5" s="15"/>
+      <c r="ALN5" s="15"/>
+      <c r="ALO5" s="15"/>
+      <c r="ALP5" s="15"/>
+      <c r="ALQ5" s="15"/>
+      <c r="ALR5" s="15"/>
+      <c r="ALS5" s="15"/>
+      <c r="ALT5" s="15"/>
+      <c r="ALU5" s="15"/>
+      <c r="ALV5" s="15"/>
+      <c r="ALW5" s="15"/>
+      <c r="ALX5" s="15"/>
+      <c r="ALY5" s="15"/>
+      <c r="ALZ5" s="15"/>
+      <c r="AMA5" s="15"/>
+      <c r="AMB5" s="15"/>
+      <c r="AMC5" s="15"/>
+      <c r="AMD5" s="15"/>
+      <c r="AME5" s="15"/>
+      <c r="AMF5" s="15"/>
+      <c r="AMG5" s="15"/>
+      <c r="AMH5" s="15"/>
+      <c r="AMI5" s="15"/>
+      <c r="AMJ5" s="15"/>
+      <c r="AMK5" s="15"/>
+      <c r="AML5" s="15"/>
+      <c r="AMM5" s="15"/>
     </row>
-    <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
@@ -3046,7 +4070,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -3087,7 +4111,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3125,7 +4149,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1027" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
@@ -3163,7 +4187,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1027" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
@@ -3201,7 +4225,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>57</v>
       </c>
@@ -3236,7 +4260,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>63</v>
       </c>
@@ -3271,7 +4295,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>67</v>
       </c>
@@ -3306,7 +4330,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1027" ht="240" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>72</v>
       </c>
@@ -3347,7 +4371,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1027" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>337</v>
       </c>
@@ -3385,7 +4409,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>79</v>
       </c>
@@ -4050,119 +5074,3175 @@
       </c>
       <c r="AMN33" s="7"/>
     </row>
-    <row r="34" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:1028" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>468</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="15" t="s">
         <v>472</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="15" t="s">
         <v>473</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="21" t="s">
         <v>457</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="J34" s="9" t="s">
+      <c r="G34" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>565</v>
+      </c>
+      <c r="I34" s="18">
+        <v>45657</v>
+      </c>
+      <c r="J34" s="19" t="s">
         <v>474</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="10" t="s">
+      <c r="L34" s="23"/>
+      <c r="M34" s="17" t="s">
         <v>476</v>
       </c>
-      <c r="O34" s="10" t="s">
+      <c r="N34" s="15"/>
+      <c r="O34" s="17" t="s">
         <v>530</v>
       </c>
-      <c r="AMN34" s="7"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
+      <c r="AC34" s="15"/>
+      <c r="AD34" s="15"/>
+      <c r="AE34" s="15"/>
+      <c r="AF34" s="15"/>
+      <c r="AG34" s="15"/>
+      <c r="AH34" s="15"/>
+      <c r="AI34" s="15"/>
+      <c r="AJ34" s="15"/>
+      <c r="AK34" s="15"/>
+      <c r="AL34" s="15"/>
+      <c r="AM34" s="15"/>
+      <c r="AN34" s="15"/>
+      <c r="AO34" s="15"/>
+      <c r="AP34" s="15"/>
+      <c r="AQ34" s="15"/>
+      <c r="AR34" s="15"/>
+      <c r="AS34" s="15"/>
+      <c r="AT34" s="15"/>
+      <c r="AU34" s="15"/>
+      <c r="AV34" s="15"/>
+      <c r="AW34" s="15"/>
+      <c r="AX34" s="15"/>
+      <c r="AY34" s="15"/>
+      <c r="AZ34" s="15"/>
+      <c r="BA34" s="15"/>
+      <c r="BB34" s="15"/>
+      <c r="BC34" s="15"/>
+      <c r="BD34" s="15"/>
+      <c r="BE34" s="15"/>
+      <c r="BF34" s="15"/>
+      <c r="BG34" s="15"/>
+      <c r="BH34" s="15"/>
+      <c r="BI34" s="15"/>
+      <c r="BJ34" s="15"/>
+      <c r="BK34" s="15"/>
+      <c r="BL34" s="15"/>
+      <c r="BM34" s="15"/>
+      <c r="BN34" s="15"/>
+      <c r="BO34" s="15"/>
+      <c r="BP34" s="15"/>
+      <c r="BQ34" s="15"/>
+      <c r="BR34" s="15"/>
+      <c r="BS34" s="15"/>
+      <c r="BT34" s="15"/>
+      <c r="BU34" s="15"/>
+      <c r="BV34" s="15"/>
+      <c r="BW34" s="15"/>
+      <c r="BX34" s="15"/>
+      <c r="BY34" s="15"/>
+      <c r="BZ34" s="15"/>
+      <c r="CA34" s="15"/>
+      <c r="CB34" s="15"/>
+      <c r="CC34" s="15"/>
+      <c r="CD34" s="15"/>
+      <c r="CE34" s="15"/>
+      <c r="CF34" s="15"/>
+      <c r="CG34" s="15"/>
+      <c r="CH34" s="15"/>
+      <c r="CI34" s="15"/>
+      <c r="CJ34" s="15"/>
+      <c r="CK34" s="15"/>
+      <c r="CL34" s="15"/>
+      <c r="CM34" s="15"/>
+      <c r="CN34" s="15"/>
+      <c r="CO34" s="15"/>
+      <c r="CP34" s="15"/>
+      <c r="CQ34" s="15"/>
+      <c r="CR34" s="15"/>
+      <c r="CS34" s="15"/>
+      <c r="CT34" s="15"/>
+      <c r="CU34" s="15"/>
+      <c r="CV34" s="15"/>
+      <c r="CW34" s="15"/>
+      <c r="CX34" s="15"/>
+      <c r="CY34" s="15"/>
+      <c r="CZ34" s="15"/>
+      <c r="DA34" s="15"/>
+      <c r="DB34" s="15"/>
+      <c r="DC34" s="15"/>
+      <c r="DD34" s="15"/>
+      <c r="DE34" s="15"/>
+      <c r="DF34" s="15"/>
+      <c r="DG34" s="15"/>
+      <c r="DH34" s="15"/>
+      <c r="DI34" s="15"/>
+      <c r="DJ34" s="15"/>
+      <c r="DK34" s="15"/>
+      <c r="DL34" s="15"/>
+      <c r="DM34" s="15"/>
+      <c r="DN34" s="15"/>
+      <c r="DO34" s="15"/>
+      <c r="DP34" s="15"/>
+      <c r="DQ34" s="15"/>
+      <c r="DR34" s="15"/>
+      <c r="DS34" s="15"/>
+      <c r="DT34" s="15"/>
+      <c r="DU34" s="15"/>
+      <c r="DV34" s="15"/>
+      <c r="DW34" s="15"/>
+      <c r="DX34" s="15"/>
+      <c r="DY34" s="15"/>
+      <c r="DZ34" s="15"/>
+      <c r="EA34" s="15"/>
+      <c r="EB34" s="15"/>
+      <c r="EC34" s="15"/>
+      <c r="ED34" s="15"/>
+      <c r="EE34" s="15"/>
+      <c r="EF34" s="15"/>
+      <c r="EG34" s="15"/>
+      <c r="EH34" s="15"/>
+      <c r="EI34" s="15"/>
+      <c r="EJ34" s="15"/>
+      <c r="EK34" s="15"/>
+      <c r="EL34" s="15"/>
+      <c r="EM34" s="15"/>
+      <c r="EN34" s="15"/>
+      <c r="EO34" s="15"/>
+      <c r="EP34" s="15"/>
+      <c r="EQ34" s="15"/>
+      <c r="ER34" s="15"/>
+      <c r="ES34" s="15"/>
+      <c r="ET34" s="15"/>
+      <c r="EU34" s="15"/>
+      <c r="EV34" s="15"/>
+      <c r="EW34" s="15"/>
+      <c r="EX34" s="15"/>
+      <c r="EY34" s="15"/>
+      <c r="EZ34" s="15"/>
+      <c r="FA34" s="15"/>
+      <c r="FB34" s="15"/>
+      <c r="FC34" s="15"/>
+      <c r="FD34" s="15"/>
+      <c r="FE34" s="15"/>
+      <c r="FF34" s="15"/>
+      <c r="FG34" s="15"/>
+      <c r="FH34" s="15"/>
+      <c r="FI34" s="15"/>
+      <c r="FJ34" s="15"/>
+      <c r="FK34" s="15"/>
+      <c r="FL34" s="15"/>
+      <c r="FM34" s="15"/>
+      <c r="FN34" s="15"/>
+      <c r="FO34" s="15"/>
+      <c r="FP34" s="15"/>
+      <c r="FQ34" s="15"/>
+      <c r="FR34" s="15"/>
+      <c r="FS34" s="15"/>
+      <c r="FT34" s="15"/>
+      <c r="FU34" s="15"/>
+      <c r="FV34" s="15"/>
+      <c r="FW34" s="15"/>
+      <c r="FX34" s="15"/>
+      <c r="FY34" s="15"/>
+      <c r="FZ34" s="15"/>
+      <c r="GA34" s="15"/>
+      <c r="GB34" s="15"/>
+      <c r="GC34" s="15"/>
+      <c r="GD34" s="15"/>
+      <c r="GE34" s="15"/>
+      <c r="GF34" s="15"/>
+      <c r="GG34" s="15"/>
+      <c r="GH34" s="15"/>
+      <c r="GI34" s="15"/>
+      <c r="GJ34" s="15"/>
+      <c r="GK34" s="15"/>
+      <c r="GL34" s="15"/>
+      <c r="GM34" s="15"/>
+      <c r="GN34" s="15"/>
+      <c r="GO34" s="15"/>
+      <c r="GP34" s="15"/>
+      <c r="GQ34" s="15"/>
+      <c r="GR34" s="15"/>
+      <c r="GS34" s="15"/>
+      <c r="GT34" s="15"/>
+      <c r="GU34" s="15"/>
+      <c r="GV34" s="15"/>
+      <c r="GW34" s="15"/>
+      <c r="GX34" s="15"/>
+      <c r="GY34" s="15"/>
+      <c r="GZ34" s="15"/>
+      <c r="HA34" s="15"/>
+      <c r="HB34" s="15"/>
+      <c r="HC34" s="15"/>
+      <c r="HD34" s="15"/>
+      <c r="HE34" s="15"/>
+      <c r="HF34" s="15"/>
+      <c r="HG34" s="15"/>
+      <c r="HH34" s="15"/>
+      <c r="HI34" s="15"/>
+      <c r="HJ34" s="15"/>
+      <c r="HK34" s="15"/>
+      <c r="HL34" s="15"/>
+      <c r="HM34" s="15"/>
+      <c r="HN34" s="15"/>
+      <c r="HO34" s="15"/>
+      <c r="HP34" s="15"/>
+      <c r="HQ34" s="15"/>
+      <c r="HR34" s="15"/>
+      <c r="HS34" s="15"/>
+      <c r="HT34" s="15"/>
+      <c r="HU34" s="15"/>
+      <c r="HV34" s="15"/>
+      <c r="HW34" s="15"/>
+      <c r="HX34" s="15"/>
+      <c r="HY34" s="15"/>
+      <c r="HZ34" s="15"/>
+      <c r="IA34" s="15"/>
+      <c r="IB34" s="15"/>
+      <c r="IC34" s="15"/>
+      <c r="ID34" s="15"/>
+      <c r="IE34" s="15"/>
+      <c r="IF34" s="15"/>
+      <c r="IG34" s="15"/>
+      <c r="IH34" s="15"/>
+      <c r="II34" s="15"/>
+      <c r="IJ34" s="15"/>
+      <c r="IK34" s="15"/>
+      <c r="IL34" s="15"/>
+      <c r="IM34" s="15"/>
+      <c r="IN34" s="15"/>
+      <c r="IO34" s="15"/>
+      <c r="IP34" s="15"/>
+      <c r="IQ34" s="15"/>
+      <c r="IR34" s="15"/>
+      <c r="IS34" s="15"/>
+      <c r="IT34" s="15"/>
+      <c r="IU34" s="15"/>
+      <c r="IV34" s="15"/>
+      <c r="IW34" s="15"/>
+      <c r="IX34" s="15"/>
+      <c r="IY34" s="15"/>
+      <c r="IZ34" s="15"/>
+      <c r="JA34" s="15"/>
+      <c r="JB34" s="15"/>
+      <c r="JC34" s="15"/>
+      <c r="JD34" s="15"/>
+      <c r="JE34" s="15"/>
+      <c r="JF34" s="15"/>
+      <c r="JG34" s="15"/>
+      <c r="JH34" s="15"/>
+      <c r="JI34" s="15"/>
+      <c r="JJ34" s="15"/>
+      <c r="JK34" s="15"/>
+      <c r="JL34" s="15"/>
+      <c r="JM34" s="15"/>
+      <c r="JN34" s="15"/>
+      <c r="JO34" s="15"/>
+      <c r="JP34" s="15"/>
+      <c r="JQ34" s="15"/>
+      <c r="JR34" s="15"/>
+      <c r="JS34" s="15"/>
+      <c r="JT34" s="15"/>
+      <c r="JU34" s="15"/>
+      <c r="JV34" s="15"/>
+      <c r="JW34" s="15"/>
+      <c r="JX34" s="15"/>
+      <c r="JY34" s="15"/>
+      <c r="JZ34" s="15"/>
+      <c r="KA34" s="15"/>
+      <c r="KB34" s="15"/>
+      <c r="KC34" s="15"/>
+      <c r="KD34" s="15"/>
+      <c r="KE34" s="15"/>
+      <c r="KF34" s="15"/>
+      <c r="KG34" s="15"/>
+      <c r="KH34" s="15"/>
+      <c r="KI34" s="15"/>
+      <c r="KJ34" s="15"/>
+      <c r="KK34" s="15"/>
+      <c r="KL34" s="15"/>
+      <c r="KM34" s="15"/>
+      <c r="KN34" s="15"/>
+      <c r="KO34" s="15"/>
+      <c r="KP34" s="15"/>
+      <c r="KQ34" s="15"/>
+      <c r="KR34" s="15"/>
+      <c r="KS34" s="15"/>
+      <c r="KT34" s="15"/>
+      <c r="KU34" s="15"/>
+      <c r="KV34" s="15"/>
+      <c r="KW34" s="15"/>
+      <c r="KX34" s="15"/>
+      <c r="KY34" s="15"/>
+      <c r="KZ34" s="15"/>
+      <c r="LA34" s="15"/>
+      <c r="LB34" s="15"/>
+      <c r="LC34" s="15"/>
+      <c r="LD34" s="15"/>
+      <c r="LE34" s="15"/>
+      <c r="LF34" s="15"/>
+      <c r="LG34" s="15"/>
+      <c r="LH34" s="15"/>
+      <c r="LI34" s="15"/>
+      <c r="LJ34" s="15"/>
+      <c r="LK34" s="15"/>
+      <c r="LL34" s="15"/>
+      <c r="LM34" s="15"/>
+      <c r="LN34" s="15"/>
+      <c r="LO34" s="15"/>
+      <c r="LP34" s="15"/>
+      <c r="LQ34" s="15"/>
+      <c r="LR34" s="15"/>
+      <c r="LS34" s="15"/>
+      <c r="LT34" s="15"/>
+      <c r="LU34" s="15"/>
+      <c r="LV34" s="15"/>
+      <c r="LW34" s="15"/>
+      <c r="LX34" s="15"/>
+      <c r="LY34" s="15"/>
+      <c r="LZ34" s="15"/>
+      <c r="MA34" s="15"/>
+      <c r="MB34" s="15"/>
+      <c r="MC34" s="15"/>
+      <c r="MD34" s="15"/>
+      <c r="ME34" s="15"/>
+      <c r="MF34" s="15"/>
+      <c r="MG34" s="15"/>
+      <c r="MH34" s="15"/>
+      <c r="MI34" s="15"/>
+      <c r="MJ34" s="15"/>
+      <c r="MK34" s="15"/>
+      <c r="ML34" s="15"/>
+      <c r="MM34" s="15"/>
+      <c r="MN34" s="15"/>
+      <c r="MO34" s="15"/>
+      <c r="MP34" s="15"/>
+      <c r="MQ34" s="15"/>
+      <c r="MR34" s="15"/>
+      <c r="MS34" s="15"/>
+      <c r="MT34" s="15"/>
+      <c r="MU34" s="15"/>
+      <c r="MV34" s="15"/>
+      <c r="MW34" s="15"/>
+      <c r="MX34" s="15"/>
+      <c r="MY34" s="15"/>
+      <c r="MZ34" s="15"/>
+      <c r="NA34" s="15"/>
+      <c r="NB34" s="15"/>
+      <c r="NC34" s="15"/>
+      <c r="ND34" s="15"/>
+      <c r="NE34" s="15"/>
+      <c r="NF34" s="15"/>
+      <c r="NG34" s="15"/>
+      <c r="NH34" s="15"/>
+      <c r="NI34" s="15"/>
+      <c r="NJ34" s="15"/>
+      <c r="NK34" s="15"/>
+      <c r="NL34" s="15"/>
+      <c r="NM34" s="15"/>
+      <c r="NN34" s="15"/>
+      <c r="NO34" s="15"/>
+      <c r="NP34" s="15"/>
+      <c r="NQ34" s="15"/>
+      <c r="NR34" s="15"/>
+      <c r="NS34" s="15"/>
+      <c r="NT34" s="15"/>
+      <c r="NU34" s="15"/>
+      <c r="NV34" s="15"/>
+      <c r="NW34" s="15"/>
+      <c r="NX34" s="15"/>
+      <c r="NY34" s="15"/>
+      <c r="NZ34" s="15"/>
+      <c r="OA34" s="15"/>
+      <c r="OB34" s="15"/>
+      <c r="OC34" s="15"/>
+      <c r="OD34" s="15"/>
+      <c r="OE34" s="15"/>
+      <c r="OF34" s="15"/>
+      <c r="OG34" s="15"/>
+      <c r="OH34" s="15"/>
+      <c r="OI34" s="15"/>
+      <c r="OJ34" s="15"/>
+      <c r="OK34" s="15"/>
+      <c r="OL34" s="15"/>
+      <c r="OM34" s="15"/>
+      <c r="ON34" s="15"/>
+      <c r="OO34" s="15"/>
+      <c r="OP34" s="15"/>
+      <c r="OQ34" s="15"/>
+      <c r="OR34" s="15"/>
+      <c r="OS34" s="15"/>
+      <c r="OT34" s="15"/>
+      <c r="OU34" s="15"/>
+      <c r="OV34" s="15"/>
+      <c r="OW34" s="15"/>
+      <c r="OX34" s="15"/>
+      <c r="OY34" s="15"/>
+      <c r="OZ34" s="15"/>
+      <c r="PA34" s="15"/>
+      <c r="PB34" s="15"/>
+      <c r="PC34" s="15"/>
+      <c r="PD34" s="15"/>
+      <c r="PE34" s="15"/>
+      <c r="PF34" s="15"/>
+      <c r="PG34" s="15"/>
+      <c r="PH34" s="15"/>
+      <c r="PI34" s="15"/>
+      <c r="PJ34" s="15"/>
+      <c r="PK34" s="15"/>
+      <c r="PL34" s="15"/>
+      <c r="PM34" s="15"/>
+      <c r="PN34" s="15"/>
+      <c r="PO34" s="15"/>
+      <c r="PP34" s="15"/>
+      <c r="PQ34" s="15"/>
+      <c r="PR34" s="15"/>
+      <c r="PS34" s="15"/>
+      <c r="PT34" s="15"/>
+      <c r="PU34" s="15"/>
+      <c r="PV34" s="15"/>
+      <c r="PW34" s="15"/>
+      <c r="PX34" s="15"/>
+      <c r="PY34" s="15"/>
+      <c r="PZ34" s="15"/>
+      <c r="QA34" s="15"/>
+      <c r="QB34" s="15"/>
+      <c r="QC34" s="15"/>
+      <c r="QD34" s="15"/>
+      <c r="QE34" s="15"/>
+      <c r="QF34" s="15"/>
+      <c r="QG34" s="15"/>
+      <c r="QH34" s="15"/>
+      <c r="QI34" s="15"/>
+      <c r="QJ34" s="15"/>
+      <c r="QK34" s="15"/>
+      <c r="QL34" s="15"/>
+      <c r="QM34" s="15"/>
+      <c r="QN34" s="15"/>
+      <c r="QO34" s="15"/>
+      <c r="QP34" s="15"/>
+      <c r="QQ34" s="15"/>
+      <c r="QR34" s="15"/>
+      <c r="QS34" s="15"/>
+      <c r="QT34" s="15"/>
+      <c r="QU34" s="15"/>
+      <c r="QV34" s="15"/>
+      <c r="QW34" s="15"/>
+      <c r="QX34" s="15"/>
+      <c r="QY34" s="15"/>
+      <c r="QZ34" s="15"/>
+      <c r="RA34" s="15"/>
+      <c r="RB34" s="15"/>
+      <c r="RC34" s="15"/>
+      <c r="RD34" s="15"/>
+      <c r="RE34" s="15"/>
+      <c r="RF34" s="15"/>
+      <c r="RG34" s="15"/>
+      <c r="RH34" s="15"/>
+      <c r="RI34" s="15"/>
+      <c r="RJ34" s="15"/>
+      <c r="RK34" s="15"/>
+      <c r="RL34" s="15"/>
+      <c r="RM34" s="15"/>
+      <c r="RN34" s="15"/>
+      <c r="RO34" s="15"/>
+      <c r="RP34" s="15"/>
+      <c r="RQ34" s="15"/>
+      <c r="RR34" s="15"/>
+      <c r="RS34" s="15"/>
+      <c r="RT34" s="15"/>
+      <c r="RU34" s="15"/>
+      <c r="RV34" s="15"/>
+      <c r="RW34" s="15"/>
+      <c r="RX34" s="15"/>
+      <c r="RY34" s="15"/>
+      <c r="RZ34" s="15"/>
+      <c r="SA34" s="15"/>
+      <c r="SB34" s="15"/>
+      <c r="SC34" s="15"/>
+      <c r="SD34" s="15"/>
+      <c r="SE34" s="15"/>
+      <c r="SF34" s="15"/>
+      <c r="SG34" s="15"/>
+      <c r="SH34" s="15"/>
+      <c r="SI34" s="15"/>
+      <c r="SJ34" s="15"/>
+      <c r="SK34" s="15"/>
+      <c r="SL34" s="15"/>
+      <c r="SM34" s="15"/>
+      <c r="SN34" s="15"/>
+      <c r="SO34" s="15"/>
+      <c r="SP34" s="15"/>
+      <c r="SQ34" s="15"/>
+      <c r="SR34" s="15"/>
+      <c r="SS34" s="15"/>
+      <c r="ST34" s="15"/>
+      <c r="SU34" s="15"/>
+      <c r="SV34" s="15"/>
+      <c r="SW34" s="15"/>
+      <c r="SX34" s="15"/>
+      <c r="SY34" s="15"/>
+      <c r="SZ34" s="15"/>
+      <c r="TA34" s="15"/>
+      <c r="TB34" s="15"/>
+      <c r="TC34" s="15"/>
+      <c r="TD34" s="15"/>
+      <c r="TE34" s="15"/>
+      <c r="TF34" s="15"/>
+      <c r="TG34" s="15"/>
+      <c r="TH34" s="15"/>
+      <c r="TI34" s="15"/>
+      <c r="TJ34" s="15"/>
+      <c r="TK34" s="15"/>
+      <c r="TL34" s="15"/>
+      <c r="TM34" s="15"/>
+      <c r="TN34" s="15"/>
+      <c r="TO34" s="15"/>
+      <c r="TP34" s="15"/>
+      <c r="TQ34" s="15"/>
+      <c r="TR34" s="15"/>
+      <c r="TS34" s="15"/>
+      <c r="TT34" s="15"/>
+      <c r="TU34" s="15"/>
+      <c r="TV34" s="15"/>
+      <c r="TW34" s="15"/>
+      <c r="TX34" s="15"/>
+      <c r="TY34" s="15"/>
+      <c r="TZ34" s="15"/>
+      <c r="UA34" s="15"/>
+      <c r="UB34" s="15"/>
+      <c r="UC34" s="15"/>
+      <c r="UD34" s="15"/>
+      <c r="UE34" s="15"/>
+      <c r="UF34" s="15"/>
+      <c r="UG34" s="15"/>
+      <c r="UH34" s="15"/>
+      <c r="UI34" s="15"/>
+      <c r="UJ34" s="15"/>
+      <c r="UK34" s="15"/>
+      <c r="UL34" s="15"/>
+      <c r="UM34" s="15"/>
+      <c r="UN34" s="15"/>
+      <c r="UO34" s="15"/>
+      <c r="UP34" s="15"/>
+      <c r="UQ34" s="15"/>
+      <c r="UR34" s="15"/>
+      <c r="US34" s="15"/>
+      <c r="UT34" s="15"/>
+      <c r="UU34" s="15"/>
+      <c r="UV34" s="15"/>
+      <c r="UW34" s="15"/>
+      <c r="UX34" s="15"/>
+      <c r="UY34" s="15"/>
+      <c r="UZ34" s="15"/>
+      <c r="VA34" s="15"/>
+      <c r="VB34" s="15"/>
+      <c r="VC34" s="15"/>
+      <c r="VD34" s="15"/>
+      <c r="VE34" s="15"/>
+      <c r="VF34" s="15"/>
+      <c r="VG34" s="15"/>
+      <c r="VH34" s="15"/>
+      <c r="VI34" s="15"/>
+      <c r="VJ34" s="15"/>
+      <c r="VK34" s="15"/>
+      <c r="VL34" s="15"/>
+      <c r="VM34" s="15"/>
+      <c r="VN34" s="15"/>
+      <c r="VO34" s="15"/>
+      <c r="VP34" s="15"/>
+      <c r="VQ34" s="15"/>
+      <c r="VR34" s="15"/>
+      <c r="VS34" s="15"/>
+      <c r="VT34" s="15"/>
+      <c r="VU34" s="15"/>
+      <c r="VV34" s="15"/>
+      <c r="VW34" s="15"/>
+      <c r="VX34" s="15"/>
+      <c r="VY34" s="15"/>
+      <c r="VZ34" s="15"/>
+      <c r="WA34" s="15"/>
+      <c r="WB34" s="15"/>
+      <c r="WC34" s="15"/>
+      <c r="WD34" s="15"/>
+      <c r="WE34" s="15"/>
+      <c r="WF34" s="15"/>
+      <c r="WG34" s="15"/>
+      <c r="WH34" s="15"/>
+      <c r="WI34" s="15"/>
+      <c r="WJ34" s="15"/>
+      <c r="WK34" s="15"/>
+      <c r="WL34" s="15"/>
+      <c r="WM34" s="15"/>
+      <c r="WN34" s="15"/>
+      <c r="WO34" s="15"/>
+      <c r="WP34" s="15"/>
+      <c r="WQ34" s="15"/>
+      <c r="WR34" s="15"/>
+      <c r="WS34" s="15"/>
+      <c r="WT34" s="15"/>
+      <c r="WU34" s="15"/>
+      <c r="WV34" s="15"/>
+      <c r="WW34" s="15"/>
+      <c r="WX34" s="15"/>
+      <c r="WY34" s="15"/>
+      <c r="WZ34" s="15"/>
+      <c r="XA34" s="15"/>
+      <c r="XB34" s="15"/>
+      <c r="XC34" s="15"/>
+      <c r="XD34" s="15"/>
+      <c r="XE34" s="15"/>
+      <c r="XF34" s="15"/>
+      <c r="XG34" s="15"/>
+      <c r="XH34" s="15"/>
+      <c r="XI34" s="15"/>
+      <c r="XJ34" s="15"/>
+      <c r="XK34" s="15"/>
+      <c r="XL34" s="15"/>
+      <c r="XM34" s="15"/>
+      <c r="XN34" s="15"/>
+      <c r="XO34" s="15"/>
+      <c r="XP34" s="15"/>
+      <c r="XQ34" s="15"/>
+      <c r="XR34" s="15"/>
+      <c r="XS34" s="15"/>
+      <c r="XT34" s="15"/>
+      <c r="XU34" s="15"/>
+      <c r="XV34" s="15"/>
+      <c r="XW34" s="15"/>
+      <c r="XX34" s="15"/>
+      <c r="XY34" s="15"/>
+      <c r="XZ34" s="15"/>
+      <c r="YA34" s="15"/>
+      <c r="YB34" s="15"/>
+      <c r="YC34" s="15"/>
+      <c r="YD34" s="15"/>
+      <c r="YE34" s="15"/>
+      <c r="YF34" s="15"/>
+      <c r="YG34" s="15"/>
+      <c r="YH34" s="15"/>
+      <c r="YI34" s="15"/>
+      <c r="YJ34" s="15"/>
+      <c r="YK34" s="15"/>
+      <c r="YL34" s="15"/>
+      <c r="YM34" s="15"/>
+      <c r="YN34" s="15"/>
+      <c r="YO34" s="15"/>
+      <c r="YP34" s="15"/>
+      <c r="YQ34" s="15"/>
+      <c r="YR34" s="15"/>
+      <c r="YS34" s="15"/>
+      <c r="YT34" s="15"/>
+      <c r="YU34" s="15"/>
+      <c r="YV34" s="15"/>
+      <c r="YW34" s="15"/>
+      <c r="YX34" s="15"/>
+      <c r="YY34" s="15"/>
+      <c r="YZ34" s="15"/>
+      <c r="ZA34" s="15"/>
+      <c r="ZB34" s="15"/>
+      <c r="ZC34" s="15"/>
+      <c r="ZD34" s="15"/>
+      <c r="ZE34" s="15"/>
+      <c r="ZF34" s="15"/>
+      <c r="ZG34" s="15"/>
+      <c r="ZH34" s="15"/>
+      <c r="ZI34" s="15"/>
+      <c r="ZJ34" s="15"/>
+      <c r="ZK34" s="15"/>
+      <c r="ZL34" s="15"/>
+      <c r="ZM34" s="15"/>
+      <c r="ZN34" s="15"/>
+      <c r="ZO34" s="15"/>
+      <c r="ZP34" s="15"/>
+      <c r="ZQ34" s="15"/>
+      <c r="ZR34" s="15"/>
+      <c r="ZS34" s="15"/>
+      <c r="ZT34" s="15"/>
+      <c r="ZU34" s="15"/>
+      <c r="ZV34" s="15"/>
+      <c r="ZW34" s="15"/>
+      <c r="ZX34" s="15"/>
+      <c r="ZY34" s="15"/>
+      <c r="ZZ34" s="15"/>
+      <c r="AAA34" s="15"/>
+      <c r="AAB34" s="15"/>
+      <c r="AAC34" s="15"/>
+      <c r="AAD34" s="15"/>
+      <c r="AAE34" s="15"/>
+      <c r="AAF34" s="15"/>
+      <c r="AAG34" s="15"/>
+      <c r="AAH34" s="15"/>
+      <c r="AAI34" s="15"/>
+      <c r="AAJ34" s="15"/>
+      <c r="AAK34" s="15"/>
+      <c r="AAL34" s="15"/>
+      <c r="AAM34" s="15"/>
+      <c r="AAN34" s="15"/>
+      <c r="AAO34" s="15"/>
+      <c r="AAP34" s="15"/>
+      <c r="AAQ34" s="15"/>
+      <c r="AAR34" s="15"/>
+      <c r="AAS34" s="15"/>
+      <c r="AAT34" s="15"/>
+      <c r="AAU34" s="15"/>
+      <c r="AAV34" s="15"/>
+      <c r="AAW34" s="15"/>
+      <c r="AAX34" s="15"/>
+      <c r="AAY34" s="15"/>
+      <c r="AAZ34" s="15"/>
+      <c r="ABA34" s="15"/>
+      <c r="ABB34" s="15"/>
+      <c r="ABC34" s="15"/>
+      <c r="ABD34" s="15"/>
+      <c r="ABE34" s="15"/>
+      <c r="ABF34" s="15"/>
+      <c r="ABG34" s="15"/>
+      <c r="ABH34" s="15"/>
+      <c r="ABI34" s="15"/>
+      <c r="ABJ34" s="15"/>
+      <c r="ABK34" s="15"/>
+      <c r="ABL34" s="15"/>
+      <c r="ABM34" s="15"/>
+      <c r="ABN34" s="15"/>
+      <c r="ABO34" s="15"/>
+      <c r="ABP34" s="15"/>
+      <c r="ABQ34" s="15"/>
+      <c r="ABR34" s="15"/>
+      <c r="ABS34" s="15"/>
+      <c r="ABT34" s="15"/>
+      <c r="ABU34" s="15"/>
+      <c r="ABV34" s="15"/>
+      <c r="ABW34" s="15"/>
+      <c r="ABX34" s="15"/>
+      <c r="ABY34" s="15"/>
+      <c r="ABZ34" s="15"/>
+      <c r="ACA34" s="15"/>
+      <c r="ACB34" s="15"/>
+      <c r="ACC34" s="15"/>
+      <c r="ACD34" s="15"/>
+      <c r="ACE34" s="15"/>
+      <c r="ACF34" s="15"/>
+      <c r="ACG34" s="15"/>
+      <c r="ACH34" s="15"/>
+      <c r="ACI34" s="15"/>
+      <c r="ACJ34" s="15"/>
+      <c r="ACK34" s="15"/>
+      <c r="ACL34" s="15"/>
+      <c r="ACM34" s="15"/>
+      <c r="ACN34" s="15"/>
+      <c r="ACO34" s="15"/>
+      <c r="ACP34" s="15"/>
+      <c r="ACQ34" s="15"/>
+      <c r="ACR34" s="15"/>
+      <c r="ACS34" s="15"/>
+      <c r="ACT34" s="15"/>
+      <c r="ACU34" s="15"/>
+      <c r="ACV34" s="15"/>
+      <c r="ACW34" s="15"/>
+      <c r="ACX34" s="15"/>
+      <c r="ACY34" s="15"/>
+      <c r="ACZ34" s="15"/>
+      <c r="ADA34" s="15"/>
+      <c r="ADB34" s="15"/>
+      <c r="ADC34" s="15"/>
+      <c r="ADD34" s="15"/>
+      <c r="ADE34" s="15"/>
+      <c r="ADF34" s="15"/>
+      <c r="ADG34" s="15"/>
+      <c r="ADH34" s="15"/>
+      <c r="ADI34" s="15"/>
+      <c r="ADJ34" s="15"/>
+      <c r="ADK34" s="15"/>
+      <c r="ADL34" s="15"/>
+      <c r="ADM34" s="15"/>
+      <c r="ADN34" s="15"/>
+      <c r="ADO34" s="15"/>
+      <c r="ADP34" s="15"/>
+      <c r="ADQ34" s="15"/>
+      <c r="ADR34" s="15"/>
+      <c r="ADS34" s="15"/>
+      <c r="ADT34" s="15"/>
+      <c r="ADU34" s="15"/>
+      <c r="ADV34" s="15"/>
+      <c r="ADW34" s="15"/>
+      <c r="ADX34" s="15"/>
+      <c r="ADY34" s="15"/>
+      <c r="ADZ34" s="15"/>
+      <c r="AEA34" s="15"/>
+      <c r="AEB34" s="15"/>
+      <c r="AEC34" s="15"/>
+      <c r="AED34" s="15"/>
+      <c r="AEE34" s="15"/>
+      <c r="AEF34" s="15"/>
+      <c r="AEG34" s="15"/>
+      <c r="AEH34" s="15"/>
+      <c r="AEI34" s="15"/>
+      <c r="AEJ34" s="15"/>
+      <c r="AEK34" s="15"/>
+      <c r="AEL34" s="15"/>
+      <c r="AEM34" s="15"/>
+      <c r="AEN34" s="15"/>
+      <c r="AEO34" s="15"/>
+      <c r="AEP34" s="15"/>
+      <c r="AEQ34" s="15"/>
+      <c r="AER34" s="15"/>
+      <c r="AES34" s="15"/>
+      <c r="AET34" s="15"/>
+      <c r="AEU34" s="15"/>
+      <c r="AEV34" s="15"/>
+      <c r="AEW34" s="15"/>
+      <c r="AEX34" s="15"/>
+      <c r="AEY34" s="15"/>
+      <c r="AEZ34" s="15"/>
+      <c r="AFA34" s="15"/>
+      <c r="AFB34" s="15"/>
+      <c r="AFC34" s="15"/>
+      <c r="AFD34" s="15"/>
+      <c r="AFE34" s="15"/>
+      <c r="AFF34" s="15"/>
+      <c r="AFG34" s="15"/>
+      <c r="AFH34" s="15"/>
+      <c r="AFI34" s="15"/>
+      <c r="AFJ34" s="15"/>
+      <c r="AFK34" s="15"/>
+      <c r="AFL34" s="15"/>
+      <c r="AFM34" s="15"/>
+      <c r="AFN34" s="15"/>
+      <c r="AFO34" s="15"/>
+      <c r="AFP34" s="15"/>
+      <c r="AFQ34" s="15"/>
+      <c r="AFR34" s="15"/>
+      <c r="AFS34" s="15"/>
+      <c r="AFT34" s="15"/>
+      <c r="AFU34" s="15"/>
+      <c r="AFV34" s="15"/>
+      <c r="AFW34" s="15"/>
+      <c r="AFX34" s="15"/>
+      <c r="AFY34" s="15"/>
+      <c r="AFZ34" s="15"/>
+      <c r="AGA34" s="15"/>
+      <c r="AGB34" s="15"/>
+      <c r="AGC34" s="15"/>
+      <c r="AGD34" s="15"/>
+      <c r="AGE34" s="15"/>
+      <c r="AGF34" s="15"/>
+      <c r="AGG34" s="15"/>
+      <c r="AGH34" s="15"/>
+      <c r="AGI34" s="15"/>
+      <c r="AGJ34" s="15"/>
+      <c r="AGK34" s="15"/>
+      <c r="AGL34" s="15"/>
+      <c r="AGM34" s="15"/>
+      <c r="AGN34" s="15"/>
+      <c r="AGO34" s="15"/>
+      <c r="AGP34" s="15"/>
+      <c r="AGQ34" s="15"/>
+      <c r="AGR34" s="15"/>
+      <c r="AGS34" s="15"/>
+      <c r="AGT34" s="15"/>
+      <c r="AGU34" s="15"/>
+      <c r="AGV34" s="15"/>
+      <c r="AGW34" s="15"/>
+      <c r="AGX34" s="15"/>
+      <c r="AGY34" s="15"/>
+      <c r="AGZ34" s="15"/>
+      <c r="AHA34" s="15"/>
+      <c r="AHB34" s="15"/>
+      <c r="AHC34" s="15"/>
+      <c r="AHD34" s="15"/>
+      <c r="AHE34" s="15"/>
+      <c r="AHF34" s="15"/>
+      <c r="AHG34" s="15"/>
+      <c r="AHH34" s="15"/>
+      <c r="AHI34" s="15"/>
+      <c r="AHJ34" s="15"/>
+      <c r="AHK34" s="15"/>
+      <c r="AHL34" s="15"/>
+      <c r="AHM34" s="15"/>
+      <c r="AHN34" s="15"/>
+      <c r="AHO34" s="15"/>
+      <c r="AHP34" s="15"/>
+      <c r="AHQ34" s="15"/>
+      <c r="AHR34" s="15"/>
+      <c r="AHS34" s="15"/>
+      <c r="AHT34" s="15"/>
+      <c r="AHU34" s="15"/>
+      <c r="AHV34" s="15"/>
+      <c r="AHW34" s="15"/>
+      <c r="AHX34" s="15"/>
+      <c r="AHY34" s="15"/>
+      <c r="AHZ34" s="15"/>
+      <c r="AIA34" s="15"/>
+      <c r="AIB34" s="15"/>
+      <c r="AIC34" s="15"/>
+      <c r="AID34" s="15"/>
+      <c r="AIE34" s="15"/>
+      <c r="AIF34" s="15"/>
+      <c r="AIG34" s="15"/>
+      <c r="AIH34" s="15"/>
+      <c r="AII34" s="15"/>
+      <c r="AIJ34" s="15"/>
+      <c r="AIK34" s="15"/>
+      <c r="AIL34" s="15"/>
+      <c r="AIM34" s="15"/>
+      <c r="AIN34" s="15"/>
+      <c r="AIO34" s="15"/>
+      <c r="AIP34" s="15"/>
+      <c r="AIQ34" s="15"/>
+      <c r="AIR34" s="15"/>
+      <c r="AIS34" s="15"/>
+      <c r="AIT34" s="15"/>
+      <c r="AIU34" s="15"/>
+      <c r="AIV34" s="15"/>
+      <c r="AIW34" s="15"/>
+      <c r="AIX34" s="15"/>
+      <c r="AIY34" s="15"/>
+      <c r="AIZ34" s="15"/>
+      <c r="AJA34" s="15"/>
+      <c r="AJB34" s="15"/>
+      <c r="AJC34" s="15"/>
+      <c r="AJD34" s="15"/>
+      <c r="AJE34" s="15"/>
+      <c r="AJF34" s="15"/>
+      <c r="AJG34" s="15"/>
+      <c r="AJH34" s="15"/>
+      <c r="AJI34" s="15"/>
+      <c r="AJJ34" s="15"/>
+      <c r="AJK34" s="15"/>
+      <c r="AJL34" s="15"/>
+      <c r="AJM34" s="15"/>
+      <c r="AJN34" s="15"/>
+      <c r="AJO34" s="15"/>
+      <c r="AJP34" s="15"/>
+      <c r="AJQ34" s="15"/>
+      <c r="AJR34" s="15"/>
+      <c r="AJS34" s="15"/>
+      <c r="AJT34" s="15"/>
+      <c r="AJU34" s="15"/>
+      <c r="AJV34" s="15"/>
+      <c r="AJW34" s="15"/>
+      <c r="AJX34" s="15"/>
+      <c r="AJY34" s="15"/>
+      <c r="AJZ34" s="15"/>
+      <c r="AKA34" s="15"/>
+      <c r="AKB34" s="15"/>
+      <c r="AKC34" s="15"/>
+      <c r="AKD34" s="15"/>
+      <c r="AKE34" s="15"/>
+      <c r="AKF34" s="15"/>
+      <c r="AKG34" s="15"/>
+      <c r="AKH34" s="15"/>
+      <c r="AKI34" s="15"/>
+      <c r="AKJ34" s="15"/>
+      <c r="AKK34" s="15"/>
+      <c r="AKL34" s="15"/>
+      <c r="AKM34" s="15"/>
+      <c r="AKN34" s="15"/>
+      <c r="AKO34" s="15"/>
+      <c r="AKP34" s="15"/>
+      <c r="AKQ34" s="15"/>
+      <c r="AKR34" s="15"/>
+      <c r="AKS34" s="15"/>
+      <c r="AKT34" s="15"/>
+      <c r="AKU34" s="15"/>
+      <c r="AKV34" s="15"/>
+      <c r="AKW34" s="15"/>
+      <c r="AKX34" s="15"/>
+      <c r="AKY34" s="15"/>
+      <c r="AKZ34" s="15"/>
+      <c r="ALA34" s="15"/>
+      <c r="ALB34" s="15"/>
+      <c r="ALC34" s="15"/>
+      <c r="ALD34" s="15"/>
+      <c r="ALE34" s="15"/>
+      <c r="ALF34" s="15"/>
+      <c r="ALG34" s="15"/>
+      <c r="ALH34" s="15"/>
+      <c r="ALI34" s="15"/>
+      <c r="ALJ34" s="15"/>
+      <c r="ALK34" s="15"/>
+      <c r="ALL34" s="15"/>
+      <c r="ALM34" s="15"/>
+      <c r="ALN34" s="15"/>
+      <c r="ALO34" s="15"/>
+      <c r="ALP34" s="15"/>
+      <c r="ALQ34" s="15"/>
+      <c r="ALR34" s="15"/>
+      <c r="ALS34" s="15"/>
+      <c r="ALT34" s="15"/>
+      <c r="ALU34" s="15"/>
+      <c r="ALV34" s="15"/>
+      <c r="ALW34" s="15"/>
+      <c r="ALX34" s="15"/>
+      <c r="ALY34" s="15"/>
+      <c r="ALZ34" s="15"/>
+      <c r="AMA34" s="15"/>
+      <c r="AMB34" s="15"/>
+      <c r="AMC34" s="15"/>
+      <c r="AMD34" s="15"/>
+      <c r="AME34" s="15"/>
+      <c r="AMF34" s="15"/>
+      <c r="AMG34" s="15"/>
+      <c r="AMH34" s="15"/>
+      <c r="AMI34" s="15"/>
+      <c r="AMJ34" s="15"/>
+      <c r="AMK34" s="15"/>
+      <c r="AML34" s="15"/>
+      <c r="AMM34" s="15"/>
+      <c r="AMN34" s="15"/>
     </row>
-    <row r="35" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:1028" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
         <v>470</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="15" t="s">
         <v>471</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="15" t="s">
         <v>477</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="15" t="s">
         <v>473</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="21" t="s">
         <v>457</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="J35" s="9" t="s">
+      <c r="G35" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>565</v>
+      </c>
+      <c r="I35" s="18">
+        <v>45657</v>
+      </c>
+      <c r="J35" s="19" t="s">
         <v>478</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="L35" s="11"/>
-      <c r="M35" s="10" t="s">
+      <c r="L35" s="23"/>
+      <c r="M35" s="17" t="s">
         <v>480</v>
       </c>
-      <c r="O35" s="10" t="s">
+      <c r="N35" s="15"/>
+      <c r="O35" s="17" t="s">
         <v>530</v>
       </c>
-      <c r="AMN35" s="7"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+      <c r="AA35" s="15"/>
+      <c r="AB35" s="15"/>
+      <c r="AC35" s="15"/>
+      <c r="AD35" s="15"/>
+      <c r="AE35" s="15"/>
+      <c r="AF35" s="15"/>
+      <c r="AG35" s="15"/>
+      <c r="AH35" s="15"/>
+      <c r="AI35" s="15"/>
+      <c r="AJ35" s="15"/>
+      <c r="AK35" s="15"/>
+      <c r="AL35" s="15"/>
+      <c r="AM35" s="15"/>
+      <c r="AN35" s="15"/>
+      <c r="AO35" s="15"/>
+      <c r="AP35" s="15"/>
+      <c r="AQ35" s="15"/>
+      <c r="AR35" s="15"/>
+      <c r="AS35" s="15"/>
+      <c r="AT35" s="15"/>
+      <c r="AU35" s="15"/>
+      <c r="AV35" s="15"/>
+      <c r="AW35" s="15"/>
+      <c r="AX35" s="15"/>
+      <c r="AY35" s="15"/>
+      <c r="AZ35" s="15"/>
+      <c r="BA35" s="15"/>
+      <c r="BB35" s="15"/>
+      <c r="BC35" s="15"/>
+      <c r="BD35" s="15"/>
+      <c r="BE35" s="15"/>
+      <c r="BF35" s="15"/>
+      <c r="BG35" s="15"/>
+      <c r="BH35" s="15"/>
+      <c r="BI35" s="15"/>
+      <c r="BJ35" s="15"/>
+      <c r="BK35" s="15"/>
+      <c r="BL35" s="15"/>
+      <c r="BM35" s="15"/>
+      <c r="BN35" s="15"/>
+      <c r="BO35" s="15"/>
+      <c r="BP35" s="15"/>
+      <c r="BQ35" s="15"/>
+      <c r="BR35" s="15"/>
+      <c r="BS35" s="15"/>
+      <c r="BT35" s="15"/>
+      <c r="BU35" s="15"/>
+      <c r="BV35" s="15"/>
+      <c r="BW35" s="15"/>
+      <c r="BX35" s="15"/>
+      <c r="BY35" s="15"/>
+      <c r="BZ35" s="15"/>
+      <c r="CA35" s="15"/>
+      <c r="CB35" s="15"/>
+      <c r="CC35" s="15"/>
+      <c r="CD35" s="15"/>
+      <c r="CE35" s="15"/>
+      <c r="CF35" s="15"/>
+      <c r="CG35" s="15"/>
+      <c r="CH35" s="15"/>
+      <c r="CI35" s="15"/>
+      <c r="CJ35" s="15"/>
+      <c r="CK35" s="15"/>
+      <c r="CL35" s="15"/>
+      <c r="CM35" s="15"/>
+      <c r="CN35" s="15"/>
+      <c r="CO35" s="15"/>
+      <c r="CP35" s="15"/>
+      <c r="CQ35" s="15"/>
+      <c r="CR35" s="15"/>
+      <c r="CS35" s="15"/>
+      <c r="CT35" s="15"/>
+      <c r="CU35" s="15"/>
+      <c r="CV35" s="15"/>
+      <c r="CW35" s="15"/>
+      <c r="CX35" s="15"/>
+      <c r="CY35" s="15"/>
+      <c r="CZ35" s="15"/>
+      <c r="DA35" s="15"/>
+      <c r="DB35" s="15"/>
+      <c r="DC35" s="15"/>
+      <c r="DD35" s="15"/>
+      <c r="DE35" s="15"/>
+      <c r="DF35" s="15"/>
+      <c r="DG35" s="15"/>
+      <c r="DH35" s="15"/>
+      <c r="DI35" s="15"/>
+      <c r="DJ35" s="15"/>
+      <c r="DK35" s="15"/>
+      <c r="DL35" s="15"/>
+      <c r="DM35" s="15"/>
+      <c r="DN35" s="15"/>
+      <c r="DO35" s="15"/>
+      <c r="DP35" s="15"/>
+      <c r="DQ35" s="15"/>
+      <c r="DR35" s="15"/>
+      <c r="DS35" s="15"/>
+      <c r="DT35" s="15"/>
+      <c r="DU35" s="15"/>
+      <c r="DV35" s="15"/>
+      <c r="DW35" s="15"/>
+      <c r="DX35" s="15"/>
+      <c r="DY35" s="15"/>
+      <c r="DZ35" s="15"/>
+      <c r="EA35" s="15"/>
+      <c r="EB35" s="15"/>
+      <c r="EC35" s="15"/>
+      <c r="ED35" s="15"/>
+      <c r="EE35" s="15"/>
+      <c r="EF35" s="15"/>
+      <c r="EG35" s="15"/>
+      <c r="EH35" s="15"/>
+      <c r="EI35" s="15"/>
+      <c r="EJ35" s="15"/>
+      <c r="EK35" s="15"/>
+      <c r="EL35" s="15"/>
+      <c r="EM35" s="15"/>
+      <c r="EN35" s="15"/>
+      <c r="EO35" s="15"/>
+      <c r="EP35" s="15"/>
+      <c r="EQ35" s="15"/>
+      <c r="ER35" s="15"/>
+      <c r="ES35" s="15"/>
+      <c r="ET35" s="15"/>
+      <c r="EU35" s="15"/>
+      <c r="EV35" s="15"/>
+      <c r="EW35" s="15"/>
+      <c r="EX35" s="15"/>
+      <c r="EY35" s="15"/>
+      <c r="EZ35" s="15"/>
+      <c r="FA35" s="15"/>
+      <c r="FB35" s="15"/>
+      <c r="FC35" s="15"/>
+      <c r="FD35" s="15"/>
+      <c r="FE35" s="15"/>
+      <c r="FF35" s="15"/>
+      <c r="FG35" s="15"/>
+      <c r="FH35" s="15"/>
+      <c r="FI35" s="15"/>
+      <c r="FJ35" s="15"/>
+      <c r="FK35" s="15"/>
+      <c r="FL35" s="15"/>
+      <c r="FM35" s="15"/>
+      <c r="FN35" s="15"/>
+      <c r="FO35" s="15"/>
+      <c r="FP35" s="15"/>
+      <c r="FQ35" s="15"/>
+      <c r="FR35" s="15"/>
+      <c r="FS35" s="15"/>
+      <c r="FT35" s="15"/>
+      <c r="FU35" s="15"/>
+      <c r="FV35" s="15"/>
+      <c r="FW35" s="15"/>
+      <c r="FX35" s="15"/>
+      <c r="FY35" s="15"/>
+      <c r="FZ35" s="15"/>
+      <c r="GA35" s="15"/>
+      <c r="GB35" s="15"/>
+      <c r="GC35" s="15"/>
+      <c r="GD35" s="15"/>
+      <c r="GE35" s="15"/>
+      <c r="GF35" s="15"/>
+      <c r="GG35" s="15"/>
+      <c r="GH35" s="15"/>
+      <c r="GI35" s="15"/>
+      <c r="GJ35" s="15"/>
+      <c r="GK35" s="15"/>
+      <c r="GL35" s="15"/>
+      <c r="GM35" s="15"/>
+      <c r="GN35" s="15"/>
+      <c r="GO35" s="15"/>
+      <c r="GP35" s="15"/>
+      <c r="GQ35" s="15"/>
+      <c r="GR35" s="15"/>
+      <c r="GS35" s="15"/>
+      <c r="GT35" s="15"/>
+      <c r="GU35" s="15"/>
+      <c r="GV35" s="15"/>
+      <c r="GW35" s="15"/>
+      <c r="GX35" s="15"/>
+      <c r="GY35" s="15"/>
+      <c r="GZ35" s="15"/>
+      <c r="HA35" s="15"/>
+      <c r="HB35" s="15"/>
+      <c r="HC35" s="15"/>
+      <c r="HD35" s="15"/>
+      <c r="HE35" s="15"/>
+      <c r="HF35" s="15"/>
+      <c r="HG35" s="15"/>
+      <c r="HH35" s="15"/>
+      <c r="HI35" s="15"/>
+      <c r="HJ35" s="15"/>
+      <c r="HK35" s="15"/>
+      <c r="HL35" s="15"/>
+      <c r="HM35" s="15"/>
+      <c r="HN35" s="15"/>
+      <c r="HO35" s="15"/>
+      <c r="HP35" s="15"/>
+      <c r="HQ35" s="15"/>
+      <c r="HR35" s="15"/>
+      <c r="HS35" s="15"/>
+      <c r="HT35" s="15"/>
+      <c r="HU35" s="15"/>
+      <c r="HV35" s="15"/>
+      <c r="HW35" s="15"/>
+      <c r="HX35" s="15"/>
+      <c r="HY35" s="15"/>
+      <c r="HZ35" s="15"/>
+      <c r="IA35" s="15"/>
+      <c r="IB35" s="15"/>
+      <c r="IC35" s="15"/>
+      <c r="ID35" s="15"/>
+      <c r="IE35" s="15"/>
+      <c r="IF35" s="15"/>
+      <c r="IG35" s="15"/>
+      <c r="IH35" s="15"/>
+      <c r="II35" s="15"/>
+      <c r="IJ35" s="15"/>
+      <c r="IK35" s="15"/>
+      <c r="IL35" s="15"/>
+      <c r="IM35" s="15"/>
+      <c r="IN35" s="15"/>
+      <c r="IO35" s="15"/>
+      <c r="IP35" s="15"/>
+      <c r="IQ35" s="15"/>
+      <c r="IR35" s="15"/>
+      <c r="IS35" s="15"/>
+      <c r="IT35" s="15"/>
+      <c r="IU35" s="15"/>
+      <c r="IV35" s="15"/>
+      <c r="IW35" s="15"/>
+      <c r="IX35" s="15"/>
+      <c r="IY35" s="15"/>
+      <c r="IZ35" s="15"/>
+      <c r="JA35" s="15"/>
+      <c r="JB35" s="15"/>
+      <c r="JC35" s="15"/>
+      <c r="JD35" s="15"/>
+      <c r="JE35" s="15"/>
+      <c r="JF35" s="15"/>
+      <c r="JG35" s="15"/>
+      <c r="JH35" s="15"/>
+      <c r="JI35" s="15"/>
+      <c r="JJ35" s="15"/>
+      <c r="JK35" s="15"/>
+      <c r="JL35" s="15"/>
+      <c r="JM35" s="15"/>
+      <c r="JN35" s="15"/>
+      <c r="JO35" s="15"/>
+      <c r="JP35" s="15"/>
+      <c r="JQ35" s="15"/>
+      <c r="JR35" s="15"/>
+      <c r="JS35" s="15"/>
+      <c r="JT35" s="15"/>
+      <c r="JU35" s="15"/>
+      <c r="JV35" s="15"/>
+      <c r="JW35" s="15"/>
+      <c r="JX35" s="15"/>
+      <c r="JY35" s="15"/>
+      <c r="JZ35" s="15"/>
+      <c r="KA35" s="15"/>
+      <c r="KB35" s="15"/>
+      <c r="KC35" s="15"/>
+      <c r="KD35" s="15"/>
+      <c r="KE35" s="15"/>
+      <c r="KF35" s="15"/>
+      <c r="KG35" s="15"/>
+      <c r="KH35" s="15"/>
+      <c r="KI35" s="15"/>
+      <c r="KJ35" s="15"/>
+      <c r="KK35" s="15"/>
+      <c r="KL35" s="15"/>
+      <c r="KM35" s="15"/>
+      <c r="KN35" s="15"/>
+      <c r="KO35" s="15"/>
+      <c r="KP35" s="15"/>
+      <c r="KQ35" s="15"/>
+      <c r="KR35" s="15"/>
+      <c r="KS35" s="15"/>
+      <c r="KT35" s="15"/>
+      <c r="KU35" s="15"/>
+      <c r="KV35" s="15"/>
+      <c r="KW35" s="15"/>
+      <c r="KX35" s="15"/>
+      <c r="KY35" s="15"/>
+      <c r="KZ35" s="15"/>
+      <c r="LA35" s="15"/>
+      <c r="LB35" s="15"/>
+      <c r="LC35" s="15"/>
+      <c r="LD35" s="15"/>
+      <c r="LE35" s="15"/>
+      <c r="LF35" s="15"/>
+      <c r="LG35" s="15"/>
+      <c r="LH35" s="15"/>
+      <c r="LI35" s="15"/>
+      <c r="LJ35" s="15"/>
+      <c r="LK35" s="15"/>
+      <c r="LL35" s="15"/>
+      <c r="LM35" s="15"/>
+      <c r="LN35" s="15"/>
+      <c r="LO35" s="15"/>
+      <c r="LP35" s="15"/>
+      <c r="LQ35" s="15"/>
+      <c r="LR35" s="15"/>
+      <c r="LS35" s="15"/>
+      <c r="LT35" s="15"/>
+      <c r="LU35" s="15"/>
+      <c r="LV35" s="15"/>
+      <c r="LW35" s="15"/>
+      <c r="LX35" s="15"/>
+      <c r="LY35" s="15"/>
+      <c r="LZ35" s="15"/>
+      <c r="MA35" s="15"/>
+      <c r="MB35" s="15"/>
+      <c r="MC35" s="15"/>
+      <c r="MD35" s="15"/>
+      <c r="ME35" s="15"/>
+      <c r="MF35" s="15"/>
+      <c r="MG35" s="15"/>
+      <c r="MH35" s="15"/>
+      <c r="MI35" s="15"/>
+      <c r="MJ35" s="15"/>
+      <c r="MK35" s="15"/>
+      <c r="ML35" s="15"/>
+      <c r="MM35" s="15"/>
+      <c r="MN35" s="15"/>
+      <c r="MO35" s="15"/>
+      <c r="MP35" s="15"/>
+      <c r="MQ35" s="15"/>
+      <c r="MR35" s="15"/>
+      <c r="MS35" s="15"/>
+      <c r="MT35" s="15"/>
+      <c r="MU35" s="15"/>
+      <c r="MV35" s="15"/>
+      <c r="MW35" s="15"/>
+      <c r="MX35" s="15"/>
+      <c r="MY35" s="15"/>
+      <c r="MZ35" s="15"/>
+      <c r="NA35" s="15"/>
+      <c r="NB35" s="15"/>
+      <c r="NC35" s="15"/>
+      <c r="ND35" s="15"/>
+      <c r="NE35" s="15"/>
+      <c r="NF35" s="15"/>
+      <c r="NG35" s="15"/>
+      <c r="NH35" s="15"/>
+      <c r="NI35" s="15"/>
+      <c r="NJ35" s="15"/>
+      <c r="NK35" s="15"/>
+      <c r="NL35" s="15"/>
+      <c r="NM35" s="15"/>
+      <c r="NN35" s="15"/>
+      <c r="NO35" s="15"/>
+      <c r="NP35" s="15"/>
+      <c r="NQ35" s="15"/>
+      <c r="NR35" s="15"/>
+      <c r="NS35" s="15"/>
+      <c r="NT35" s="15"/>
+      <c r="NU35" s="15"/>
+      <c r="NV35" s="15"/>
+      <c r="NW35" s="15"/>
+      <c r="NX35" s="15"/>
+      <c r="NY35" s="15"/>
+      <c r="NZ35" s="15"/>
+      <c r="OA35" s="15"/>
+      <c r="OB35" s="15"/>
+      <c r="OC35" s="15"/>
+      <c r="OD35" s="15"/>
+      <c r="OE35" s="15"/>
+      <c r="OF35" s="15"/>
+      <c r="OG35" s="15"/>
+      <c r="OH35" s="15"/>
+      <c r="OI35" s="15"/>
+      <c r="OJ35" s="15"/>
+      <c r="OK35" s="15"/>
+      <c r="OL35" s="15"/>
+      <c r="OM35" s="15"/>
+      <c r="ON35" s="15"/>
+      <c r="OO35" s="15"/>
+      <c r="OP35" s="15"/>
+      <c r="OQ35" s="15"/>
+      <c r="OR35" s="15"/>
+      <c r="OS35" s="15"/>
+      <c r="OT35" s="15"/>
+      <c r="OU35" s="15"/>
+      <c r="OV35" s="15"/>
+      <c r="OW35" s="15"/>
+      <c r="OX35" s="15"/>
+      <c r="OY35" s="15"/>
+      <c r="OZ35" s="15"/>
+      <c r="PA35" s="15"/>
+      <c r="PB35" s="15"/>
+      <c r="PC35" s="15"/>
+      <c r="PD35" s="15"/>
+      <c r="PE35" s="15"/>
+      <c r="PF35" s="15"/>
+      <c r="PG35" s="15"/>
+      <c r="PH35" s="15"/>
+      <c r="PI35" s="15"/>
+      <c r="PJ35" s="15"/>
+      <c r="PK35" s="15"/>
+      <c r="PL35" s="15"/>
+      <c r="PM35" s="15"/>
+      <c r="PN35" s="15"/>
+      <c r="PO35" s="15"/>
+      <c r="PP35" s="15"/>
+      <c r="PQ35" s="15"/>
+      <c r="PR35" s="15"/>
+      <c r="PS35" s="15"/>
+      <c r="PT35" s="15"/>
+      <c r="PU35" s="15"/>
+      <c r="PV35" s="15"/>
+      <c r="PW35" s="15"/>
+      <c r="PX35" s="15"/>
+      <c r="PY35" s="15"/>
+      <c r="PZ35" s="15"/>
+      <c r="QA35" s="15"/>
+      <c r="QB35" s="15"/>
+      <c r="QC35" s="15"/>
+      <c r="QD35" s="15"/>
+      <c r="QE35" s="15"/>
+      <c r="QF35" s="15"/>
+      <c r="QG35" s="15"/>
+      <c r="QH35" s="15"/>
+      <c r="QI35" s="15"/>
+      <c r="QJ35" s="15"/>
+      <c r="QK35" s="15"/>
+      <c r="QL35" s="15"/>
+      <c r="QM35" s="15"/>
+      <c r="QN35" s="15"/>
+      <c r="QO35" s="15"/>
+      <c r="QP35" s="15"/>
+      <c r="QQ35" s="15"/>
+      <c r="QR35" s="15"/>
+      <c r="QS35" s="15"/>
+      <c r="QT35" s="15"/>
+      <c r="QU35" s="15"/>
+      <c r="QV35" s="15"/>
+      <c r="QW35" s="15"/>
+      <c r="QX35" s="15"/>
+      <c r="QY35" s="15"/>
+      <c r="QZ35" s="15"/>
+      <c r="RA35" s="15"/>
+      <c r="RB35" s="15"/>
+      <c r="RC35" s="15"/>
+      <c r="RD35" s="15"/>
+      <c r="RE35" s="15"/>
+      <c r="RF35" s="15"/>
+      <c r="RG35" s="15"/>
+      <c r="RH35" s="15"/>
+      <c r="RI35" s="15"/>
+      <c r="RJ35" s="15"/>
+      <c r="RK35" s="15"/>
+      <c r="RL35" s="15"/>
+      <c r="RM35" s="15"/>
+      <c r="RN35" s="15"/>
+      <c r="RO35" s="15"/>
+      <c r="RP35" s="15"/>
+      <c r="RQ35" s="15"/>
+      <c r="RR35" s="15"/>
+      <c r="RS35" s="15"/>
+      <c r="RT35" s="15"/>
+      <c r="RU35" s="15"/>
+      <c r="RV35" s="15"/>
+      <c r="RW35" s="15"/>
+      <c r="RX35" s="15"/>
+      <c r="RY35" s="15"/>
+      <c r="RZ35" s="15"/>
+      <c r="SA35" s="15"/>
+      <c r="SB35" s="15"/>
+      <c r="SC35" s="15"/>
+      <c r="SD35" s="15"/>
+      <c r="SE35" s="15"/>
+      <c r="SF35" s="15"/>
+      <c r="SG35" s="15"/>
+      <c r="SH35" s="15"/>
+      <c r="SI35" s="15"/>
+      <c r="SJ35" s="15"/>
+      <c r="SK35" s="15"/>
+      <c r="SL35" s="15"/>
+      <c r="SM35" s="15"/>
+      <c r="SN35" s="15"/>
+      <c r="SO35" s="15"/>
+      <c r="SP35" s="15"/>
+      <c r="SQ35" s="15"/>
+      <c r="SR35" s="15"/>
+      <c r="SS35" s="15"/>
+      <c r="ST35" s="15"/>
+      <c r="SU35" s="15"/>
+      <c r="SV35" s="15"/>
+      <c r="SW35" s="15"/>
+      <c r="SX35" s="15"/>
+      <c r="SY35" s="15"/>
+      <c r="SZ35" s="15"/>
+      <c r="TA35" s="15"/>
+      <c r="TB35" s="15"/>
+      <c r="TC35" s="15"/>
+      <c r="TD35" s="15"/>
+      <c r="TE35" s="15"/>
+      <c r="TF35" s="15"/>
+      <c r="TG35" s="15"/>
+      <c r="TH35" s="15"/>
+      <c r="TI35" s="15"/>
+      <c r="TJ35" s="15"/>
+      <c r="TK35" s="15"/>
+      <c r="TL35" s="15"/>
+      <c r="TM35" s="15"/>
+      <c r="TN35" s="15"/>
+      <c r="TO35" s="15"/>
+      <c r="TP35" s="15"/>
+      <c r="TQ35" s="15"/>
+      <c r="TR35" s="15"/>
+      <c r="TS35" s="15"/>
+      <c r="TT35" s="15"/>
+      <c r="TU35" s="15"/>
+      <c r="TV35" s="15"/>
+      <c r="TW35" s="15"/>
+      <c r="TX35" s="15"/>
+      <c r="TY35" s="15"/>
+      <c r="TZ35" s="15"/>
+      <c r="UA35" s="15"/>
+      <c r="UB35" s="15"/>
+      <c r="UC35" s="15"/>
+      <c r="UD35" s="15"/>
+      <c r="UE35" s="15"/>
+      <c r="UF35" s="15"/>
+      <c r="UG35" s="15"/>
+      <c r="UH35" s="15"/>
+      <c r="UI35" s="15"/>
+      <c r="UJ35" s="15"/>
+      <c r="UK35" s="15"/>
+      <c r="UL35" s="15"/>
+      <c r="UM35" s="15"/>
+      <c r="UN35" s="15"/>
+      <c r="UO35" s="15"/>
+      <c r="UP35" s="15"/>
+      <c r="UQ35" s="15"/>
+      <c r="UR35" s="15"/>
+      <c r="US35" s="15"/>
+      <c r="UT35" s="15"/>
+      <c r="UU35" s="15"/>
+      <c r="UV35" s="15"/>
+      <c r="UW35" s="15"/>
+      <c r="UX35" s="15"/>
+      <c r="UY35" s="15"/>
+      <c r="UZ35" s="15"/>
+      <c r="VA35" s="15"/>
+      <c r="VB35" s="15"/>
+      <c r="VC35" s="15"/>
+      <c r="VD35" s="15"/>
+      <c r="VE35" s="15"/>
+      <c r="VF35" s="15"/>
+      <c r="VG35" s="15"/>
+      <c r="VH35" s="15"/>
+      <c r="VI35" s="15"/>
+      <c r="VJ35" s="15"/>
+      <c r="VK35" s="15"/>
+      <c r="VL35" s="15"/>
+      <c r="VM35" s="15"/>
+      <c r="VN35" s="15"/>
+      <c r="VO35" s="15"/>
+      <c r="VP35" s="15"/>
+      <c r="VQ35" s="15"/>
+      <c r="VR35" s="15"/>
+      <c r="VS35" s="15"/>
+      <c r="VT35" s="15"/>
+      <c r="VU35" s="15"/>
+      <c r="VV35" s="15"/>
+      <c r="VW35" s="15"/>
+      <c r="VX35" s="15"/>
+      <c r="VY35" s="15"/>
+      <c r="VZ35" s="15"/>
+      <c r="WA35" s="15"/>
+      <c r="WB35" s="15"/>
+      <c r="WC35" s="15"/>
+      <c r="WD35" s="15"/>
+      <c r="WE35" s="15"/>
+      <c r="WF35" s="15"/>
+      <c r="WG35" s="15"/>
+      <c r="WH35" s="15"/>
+      <c r="WI35" s="15"/>
+      <c r="WJ35" s="15"/>
+      <c r="WK35" s="15"/>
+      <c r="WL35" s="15"/>
+      <c r="WM35" s="15"/>
+      <c r="WN35" s="15"/>
+      <c r="WO35" s="15"/>
+      <c r="WP35" s="15"/>
+      <c r="WQ35" s="15"/>
+      <c r="WR35" s="15"/>
+      <c r="WS35" s="15"/>
+      <c r="WT35" s="15"/>
+      <c r="WU35" s="15"/>
+      <c r="WV35" s="15"/>
+      <c r="WW35" s="15"/>
+      <c r="WX35" s="15"/>
+      <c r="WY35" s="15"/>
+      <c r="WZ35" s="15"/>
+      <c r="XA35" s="15"/>
+      <c r="XB35" s="15"/>
+      <c r="XC35" s="15"/>
+      <c r="XD35" s="15"/>
+      <c r="XE35" s="15"/>
+      <c r="XF35" s="15"/>
+      <c r="XG35" s="15"/>
+      <c r="XH35" s="15"/>
+      <c r="XI35" s="15"/>
+      <c r="XJ35" s="15"/>
+      <c r="XK35" s="15"/>
+      <c r="XL35" s="15"/>
+      <c r="XM35" s="15"/>
+      <c r="XN35" s="15"/>
+      <c r="XO35" s="15"/>
+      <c r="XP35" s="15"/>
+      <c r="XQ35" s="15"/>
+      <c r="XR35" s="15"/>
+      <c r="XS35" s="15"/>
+      <c r="XT35" s="15"/>
+      <c r="XU35" s="15"/>
+      <c r="XV35" s="15"/>
+      <c r="XW35" s="15"/>
+      <c r="XX35" s="15"/>
+      <c r="XY35" s="15"/>
+      <c r="XZ35" s="15"/>
+      <c r="YA35" s="15"/>
+      <c r="YB35" s="15"/>
+      <c r="YC35" s="15"/>
+      <c r="YD35" s="15"/>
+      <c r="YE35" s="15"/>
+      <c r="YF35" s="15"/>
+      <c r="YG35" s="15"/>
+      <c r="YH35" s="15"/>
+      <c r="YI35" s="15"/>
+      <c r="YJ35" s="15"/>
+      <c r="YK35" s="15"/>
+      <c r="YL35" s="15"/>
+      <c r="YM35" s="15"/>
+      <c r="YN35" s="15"/>
+      <c r="YO35" s="15"/>
+      <c r="YP35" s="15"/>
+      <c r="YQ35" s="15"/>
+      <c r="YR35" s="15"/>
+      <c r="YS35" s="15"/>
+      <c r="YT35" s="15"/>
+      <c r="YU35" s="15"/>
+      <c r="YV35" s="15"/>
+      <c r="YW35" s="15"/>
+      <c r="YX35" s="15"/>
+      <c r="YY35" s="15"/>
+      <c r="YZ35" s="15"/>
+      <c r="ZA35" s="15"/>
+      <c r="ZB35" s="15"/>
+      <c r="ZC35" s="15"/>
+      <c r="ZD35" s="15"/>
+      <c r="ZE35" s="15"/>
+      <c r="ZF35" s="15"/>
+      <c r="ZG35" s="15"/>
+      <c r="ZH35" s="15"/>
+      <c r="ZI35" s="15"/>
+      <c r="ZJ35" s="15"/>
+      <c r="ZK35" s="15"/>
+      <c r="ZL35" s="15"/>
+      <c r="ZM35" s="15"/>
+      <c r="ZN35" s="15"/>
+      <c r="ZO35" s="15"/>
+      <c r="ZP35" s="15"/>
+      <c r="ZQ35" s="15"/>
+      <c r="ZR35" s="15"/>
+      <c r="ZS35" s="15"/>
+      <c r="ZT35" s="15"/>
+      <c r="ZU35" s="15"/>
+      <c r="ZV35" s="15"/>
+      <c r="ZW35" s="15"/>
+      <c r="ZX35" s="15"/>
+      <c r="ZY35" s="15"/>
+      <c r="ZZ35" s="15"/>
+      <c r="AAA35" s="15"/>
+      <c r="AAB35" s="15"/>
+      <c r="AAC35" s="15"/>
+      <c r="AAD35" s="15"/>
+      <c r="AAE35" s="15"/>
+      <c r="AAF35" s="15"/>
+      <c r="AAG35" s="15"/>
+      <c r="AAH35" s="15"/>
+      <c r="AAI35" s="15"/>
+      <c r="AAJ35" s="15"/>
+      <c r="AAK35" s="15"/>
+      <c r="AAL35" s="15"/>
+      <c r="AAM35" s="15"/>
+      <c r="AAN35" s="15"/>
+      <c r="AAO35" s="15"/>
+      <c r="AAP35" s="15"/>
+      <c r="AAQ35" s="15"/>
+      <c r="AAR35" s="15"/>
+      <c r="AAS35" s="15"/>
+      <c r="AAT35" s="15"/>
+      <c r="AAU35" s="15"/>
+      <c r="AAV35" s="15"/>
+      <c r="AAW35" s="15"/>
+      <c r="AAX35" s="15"/>
+      <c r="AAY35" s="15"/>
+      <c r="AAZ35" s="15"/>
+      <c r="ABA35" s="15"/>
+      <c r="ABB35" s="15"/>
+      <c r="ABC35" s="15"/>
+      <c r="ABD35" s="15"/>
+      <c r="ABE35" s="15"/>
+      <c r="ABF35" s="15"/>
+      <c r="ABG35" s="15"/>
+      <c r="ABH35" s="15"/>
+      <c r="ABI35" s="15"/>
+      <c r="ABJ35" s="15"/>
+      <c r="ABK35" s="15"/>
+      <c r="ABL35" s="15"/>
+      <c r="ABM35" s="15"/>
+      <c r="ABN35" s="15"/>
+      <c r="ABO35" s="15"/>
+      <c r="ABP35" s="15"/>
+      <c r="ABQ35" s="15"/>
+      <c r="ABR35" s="15"/>
+      <c r="ABS35" s="15"/>
+      <c r="ABT35" s="15"/>
+      <c r="ABU35" s="15"/>
+      <c r="ABV35" s="15"/>
+      <c r="ABW35" s="15"/>
+      <c r="ABX35" s="15"/>
+      <c r="ABY35" s="15"/>
+      <c r="ABZ35" s="15"/>
+      <c r="ACA35" s="15"/>
+      <c r="ACB35" s="15"/>
+      <c r="ACC35" s="15"/>
+      <c r="ACD35" s="15"/>
+      <c r="ACE35" s="15"/>
+      <c r="ACF35" s="15"/>
+      <c r="ACG35" s="15"/>
+      <c r="ACH35" s="15"/>
+      <c r="ACI35" s="15"/>
+      <c r="ACJ35" s="15"/>
+      <c r="ACK35" s="15"/>
+      <c r="ACL35" s="15"/>
+      <c r="ACM35" s="15"/>
+      <c r="ACN35" s="15"/>
+      <c r="ACO35" s="15"/>
+      <c r="ACP35" s="15"/>
+      <c r="ACQ35" s="15"/>
+      <c r="ACR35" s="15"/>
+      <c r="ACS35" s="15"/>
+      <c r="ACT35" s="15"/>
+      <c r="ACU35" s="15"/>
+      <c r="ACV35" s="15"/>
+      <c r="ACW35" s="15"/>
+      <c r="ACX35" s="15"/>
+      <c r="ACY35" s="15"/>
+      <c r="ACZ35" s="15"/>
+      <c r="ADA35" s="15"/>
+      <c r="ADB35" s="15"/>
+      <c r="ADC35" s="15"/>
+      <c r="ADD35" s="15"/>
+      <c r="ADE35" s="15"/>
+      <c r="ADF35" s="15"/>
+      <c r="ADG35" s="15"/>
+      <c r="ADH35" s="15"/>
+      <c r="ADI35" s="15"/>
+      <c r="ADJ35" s="15"/>
+      <c r="ADK35" s="15"/>
+      <c r="ADL35" s="15"/>
+      <c r="ADM35" s="15"/>
+      <c r="ADN35" s="15"/>
+      <c r="ADO35" s="15"/>
+      <c r="ADP35" s="15"/>
+      <c r="ADQ35" s="15"/>
+      <c r="ADR35" s="15"/>
+      <c r="ADS35" s="15"/>
+      <c r="ADT35" s="15"/>
+      <c r="ADU35" s="15"/>
+      <c r="ADV35" s="15"/>
+      <c r="ADW35" s="15"/>
+      <c r="ADX35" s="15"/>
+      <c r="ADY35" s="15"/>
+      <c r="ADZ35" s="15"/>
+      <c r="AEA35" s="15"/>
+      <c r="AEB35" s="15"/>
+      <c r="AEC35" s="15"/>
+      <c r="AED35" s="15"/>
+      <c r="AEE35" s="15"/>
+      <c r="AEF35" s="15"/>
+      <c r="AEG35" s="15"/>
+      <c r="AEH35" s="15"/>
+      <c r="AEI35" s="15"/>
+      <c r="AEJ35" s="15"/>
+      <c r="AEK35" s="15"/>
+      <c r="AEL35" s="15"/>
+      <c r="AEM35" s="15"/>
+      <c r="AEN35" s="15"/>
+      <c r="AEO35" s="15"/>
+      <c r="AEP35" s="15"/>
+      <c r="AEQ35" s="15"/>
+      <c r="AER35" s="15"/>
+      <c r="AES35" s="15"/>
+      <c r="AET35" s="15"/>
+      <c r="AEU35" s="15"/>
+      <c r="AEV35" s="15"/>
+      <c r="AEW35" s="15"/>
+      <c r="AEX35" s="15"/>
+      <c r="AEY35" s="15"/>
+      <c r="AEZ35" s="15"/>
+      <c r="AFA35" s="15"/>
+      <c r="AFB35" s="15"/>
+      <c r="AFC35" s="15"/>
+      <c r="AFD35" s="15"/>
+      <c r="AFE35" s="15"/>
+      <c r="AFF35" s="15"/>
+      <c r="AFG35" s="15"/>
+      <c r="AFH35" s="15"/>
+      <c r="AFI35" s="15"/>
+      <c r="AFJ35" s="15"/>
+      <c r="AFK35" s="15"/>
+      <c r="AFL35" s="15"/>
+      <c r="AFM35" s="15"/>
+      <c r="AFN35" s="15"/>
+      <c r="AFO35" s="15"/>
+      <c r="AFP35" s="15"/>
+      <c r="AFQ35" s="15"/>
+      <c r="AFR35" s="15"/>
+      <c r="AFS35" s="15"/>
+      <c r="AFT35" s="15"/>
+      <c r="AFU35" s="15"/>
+      <c r="AFV35" s="15"/>
+      <c r="AFW35" s="15"/>
+      <c r="AFX35" s="15"/>
+      <c r="AFY35" s="15"/>
+      <c r="AFZ35" s="15"/>
+      <c r="AGA35" s="15"/>
+      <c r="AGB35" s="15"/>
+      <c r="AGC35" s="15"/>
+      <c r="AGD35" s="15"/>
+      <c r="AGE35" s="15"/>
+      <c r="AGF35" s="15"/>
+      <c r="AGG35" s="15"/>
+      <c r="AGH35" s="15"/>
+      <c r="AGI35" s="15"/>
+      <c r="AGJ35" s="15"/>
+      <c r="AGK35" s="15"/>
+      <c r="AGL35" s="15"/>
+      <c r="AGM35" s="15"/>
+      <c r="AGN35" s="15"/>
+      <c r="AGO35" s="15"/>
+      <c r="AGP35" s="15"/>
+      <c r="AGQ35" s="15"/>
+      <c r="AGR35" s="15"/>
+      <c r="AGS35" s="15"/>
+      <c r="AGT35" s="15"/>
+      <c r="AGU35" s="15"/>
+      <c r="AGV35" s="15"/>
+      <c r="AGW35" s="15"/>
+      <c r="AGX35" s="15"/>
+      <c r="AGY35" s="15"/>
+      <c r="AGZ35" s="15"/>
+      <c r="AHA35" s="15"/>
+      <c r="AHB35" s="15"/>
+      <c r="AHC35" s="15"/>
+      <c r="AHD35" s="15"/>
+      <c r="AHE35" s="15"/>
+      <c r="AHF35" s="15"/>
+      <c r="AHG35" s="15"/>
+      <c r="AHH35" s="15"/>
+      <c r="AHI35" s="15"/>
+      <c r="AHJ35" s="15"/>
+      <c r="AHK35" s="15"/>
+      <c r="AHL35" s="15"/>
+      <c r="AHM35" s="15"/>
+      <c r="AHN35" s="15"/>
+      <c r="AHO35" s="15"/>
+      <c r="AHP35" s="15"/>
+      <c r="AHQ35" s="15"/>
+      <c r="AHR35" s="15"/>
+      <c r="AHS35" s="15"/>
+      <c r="AHT35" s="15"/>
+      <c r="AHU35" s="15"/>
+      <c r="AHV35" s="15"/>
+      <c r="AHW35" s="15"/>
+      <c r="AHX35" s="15"/>
+      <c r="AHY35" s="15"/>
+      <c r="AHZ35" s="15"/>
+      <c r="AIA35" s="15"/>
+      <c r="AIB35" s="15"/>
+      <c r="AIC35" s="15"/>
+      <c r="AID35" s="15"/>
+      <c r="AIE35" s="15"/>
+      <c r="AIF35" s="15"/>
+      <c r="AIG35" s="15"/>
+      <c r="AIH35" s="15"/>
+      <c r="AII35" s="15"/>
+      <c r="AIJ35" s="15"/>
+      <c r="AIK35" s="15"/>
+      <c r="AIL35" s="15"/>
+      <c r="AIM35" s="15"/>
+      <c r="AIN35" s="15"/>
+      <c r="AIO35" s="15"/>
+      <c r="AIP35" s="15"/>
+      <c r="AIQ35" s="15"/>
+      <c r="AIR35" s="15"/>
+      <c r="AIS35" s="15"/>
+      <c r="AIT35" s="15"/>
+      <c r="AIU35" s="15"/>
+      <c r="AIV35" s="15"/>
+      <c r="AIW35" s="15"/>
+      <c r="AIX35" s="15"/>
+      <c r="AIY35" s="15"/>
+      <c r="AIZ35" s="15"/>
+      <c r="AJA35" s="15"/>
+      <c r="AJB35" s="15"/>
+      <c r="AJC35" s="15"/>
+      <c r="AJD35" s="15"/>
+      <c r="AJE35" s="15"/>
+      <c r="AJF35" s="15"/>
+      <c r="AJG35" s="15"/>
+      <c r="AJH35" s="15"/>
+      <c r="AJI35" s="15"/>
+      <c r="AJJ35" s="15"/>
+      <c r="AJK35" s="15"/>
+      <c r="AJL35" s="15"/>
+      <c r="AJM35" s="15"/>
+      <c r="AJN35" s="15"/>
+      <c r="AJO35" s="15"/>
+      <c r="AJP35" s="15"/>
+      <c r="AJQ35" s="15"/>
+      <c r="AJR35" s="15"/>
+      <c r="AJS35" s="15"/>
+      <c r="AJT35" s="15"/>
+      <c r="AJU35" s="15"/>
+      <c r="AJV35" s="15"/>
+      <c r="AJW35" s="15"/>
+      <c r="AJX35" s="15"/>
+      <c r="AJY35" s="15"/>
+      <c r="AJZ35" s="15"/>
+      <c r="AKA35" s="15"/>
+      <c r="AKB35" s="15"/>
+      <c r="AKC35" s="15"/>
+      <c r="AKD35" s="15"/>
+      <c r="AKE35" s="15"/>
+      <c r="AKF35" s="15"/>
+      <c r="AKG35" s="15"/>
+      <c r="AKH35" s="15"/>
+      <c r="AKI35" s="15"/>
+      <c r="AKJ35" s="15"/>
+      <c r="AKK35" s="15"/>
+      <c r="AKL35" s="15"/>
+      <c r="AKM35" s="15"/>
+      <c r="AKN35" s="15"/>
+      <c r="AKO35" s="15"/>
+      <c r="AKP35" s="15"/>
+      <c r="AKQ35" s="15"/>
+      <c r="AKR35" s="15"/>
+      <c r="AKS35" s="15"/>
+      <c r="AKT35" s="15"/>
+      <c r="AKU35" s="15"/>
+      <c r="AKV35" s="15"/>
+      <c r="AKW35" s="15"/>
+      <c r="AKX35" s="15"/>
+      <c r="AKY35" s="15"/>
+      <c r="AKZ35" s="15"/>
+      <c r="ALA35" s="15"/>
+      <c r="ALB35" s="15"/>
+      <c r="ALC35" s="15"/>
+      <c r="ALD35" s="15"/>
+      <c r="ALE35" s="15"/>
+      <c r="ALF35" s="15"/>
+      <c r="ALG35" s="15"/>
+      <c r="ALH35" s="15"/>
+      <c r="ALI35" s="15"/>
+      <c r="ALJ35" s="15"/>
+      <c r="ALK35" s="15"/>
+      <c r="ALL35" s="15"/>
+      <c r="ALM35" s="15"/>
+      <c r="ALN35" s="15"/>
+      <c r="ALO35" s="15"/>
+      <c r="ALP35" s="15"/>
+      <c r="ALQ35" s="15"/>
+      <c r="ALR35" s="15"/>
+      <c r="ALS35" s="15"/>
+      <c r="ALT35" s="15"/>
+      <c r="ALU35" s="15"/>
+      <c r="ALV35" s="15"/>
+      <c r="ALW35" s="15"/>
+      <c r="ALX35" s="15"/>
+      <c r="ALY35" s="15"/>
+      <c r="ALZ35" s="15"/>
+      <c r="AMA35" s="15"/>
+      <c r="AMB35" s="15"/>
+      <c r="AMC35" s="15"/>
+      <c r="AMD35" s="15"/>
+      <c r="AME35" s="15"/>
+      <c r="AMF35" s="15"/>
+      <c r="AMG35" s="15"/>
+      <c r="AMH35" s="15"/>
+      <c r="AMI35" s="15"/>
+      <c r="AMJ35" s="15"/>
+      <c r="AMK35" s="15"/>
+      <c r="AML35" s="15"/>
+      <c r="AMM35" s="15"/>
+      <c r="AMN35" s="15"/>
     </row>
-    <row r="36" spans="1:1028" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:1028" s="20" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
         <v>500</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="15" t="s">
         <v>501</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="15" t="s">
         <v>502</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="15" t="s">
         <v>503</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="J36" s="9" t="s">
+      <c r="G36" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>565</v>
+      </c>
+      <c r="I36" s="18">
+        <v>45657</v>
+      </c>
+      <c r="J36" s="19" t="s">
         <v>504</v>
       </c>
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="10" t="s">
+      <c r="L36" s="23"/>
+      <c r="M36" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="N36" s="7" t="s">
+      <c r="N36" s="15" t="s">
         <v>505</v>
       </c>
-      <c r="O36" s="10" t="s">
+      <c r="O36" s="17" t="s">
         <v>530</v>
       </c>
-      <c r="AMN36" s="7"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
+      <c r="AD36" s="15"/>
+      <c r="AE36" s="15"/>
+      <c r="AF36" s="15"/>
+      <c r="AG36" s="15"/>
+      <c r="AH36" s="15"/>
+      <c r="AI36" s="15"/>
+      <c r="AJ36" s="15"/>
+      <c r="AK36" s="15"/>
+      <c r="AL36" s="15"/>
+      <c r="AM36" s="15"/>
+      <c r="AN36" s="15"/>
+      <c r="AO36" s="15"/>
+      <c r="AP36" s="15"/>
+      <c r="AQ36" s="15"/>
+      <c r="AR36" s="15"/>
+      <c r="AS36" s="15"/>
+      <c r="AT36" s="15"/>
+      <c r="AU36" s="15"/>
+      <c r="AV36" s="15"/>
+      <c r="AW36" s="15"/>
+      <c r="AX36" s="15"/>
+      <c r="AY36" s="15"/>
+      <c r="AZ36" s="15"/>
+      <c r="BA36" s="15"/>
+      <c r="BB36" s="15"/>
+      <c r="BC36" s="15"/>
+      <c r="BD36" s="15"/>
+      <c r="BE36" s="15"/>
+      <c r="BF36" s="15"/>
+      <c r="BG36" s="15"/>
+      <c r="BH36" s="15"/>
+      <c r="BI36" s="15"/>
+      <c r="BJ36" s="15"/>
+      <c r="BK36" s="15"/>
+      <c r="BL36" s="15"/>
+      <c r="BM36" s="15"/>
+      <c r="BN36" s="15"/>
+      <c r="BO36" s="15"/>
+      <c r="BP36" s="15"/>
+      <c r="BQ36" s="15"/>
+      <c r="BR36" s="15"/>
+      <c r="BS36" s="15"/>
+      <c r="BT36" s="15"/>
+      <c r="BU36" s="15"/>
+      <c r="BV36" s="15"/>
+      <c r="BW36" s="15"/>
+      <c r="BX36" s="15"/>
+      <c r="BY36" s="15"/>
+      <c r="BZ36" s="15"/>
+      <c r="CA36" s="15"/>
+      <c r="CB36" s="15"/>
+      <c r="CC36" s="15"/>
+      <c r="CD36" s="15"/>
+      <c r="CE36" s="15"/>
+      <c r="CF36" s="15"/>
+      <c r="CG36" s="15"/>
+      <c r="CH36" s="15"/>
+      <c r="CI36" s="15"/>
+      <c r="CJ36" s="15"/>
+      <c r="CK36" s="15"/>
+      <c r="CL36" s="15"/>
+      <c r="CM36" s="15"/>
+      <c r="CN36" s="15"/>
+      <c r="CO36" s="15"/>
+      <c r="CP36" s="15"/>
+      <c r="CQ36" s="15"/>
+      <c r="CR36" s="15"/>
+      <c r="CS36" s="15"/>
+      <c r="CT36" s="15"/>
+      <c r="CU36" s="15"/>
+      <c r="CV36" s="15"/>
+      <c r="CW36" s="15"/>
+      <c r="CX36" s="15"/>
+      <c r="CY36" s="15"/>
+      <c r="CZ36" s="15"/>
+      <c r="DA36" s="15"/>
+      <c r="DB36" s="15"/>
+      <c r="DC36" s="15"/>
+      <c r="DD36" s="15"/>
+      <c r="DE36" s="15"/>
+      <c r="DF36" s="15"/>
+      <c r="DG36" s="15"/>
+      <c r="DH36" s="15"/>
+      <c r="DI36" s="15"/>
+      <c r="DJ36" s="15"/>
+      <c r="DK36" s="15"/>
+      <c r="DL36" s="15"/>
+      <c r="DM36" s="15"/>
+      <c r="DN36" s="15"/>
+      <c r="DO36" s="15"/>
+      <c r="DP36" s="15"/>
+      <c r="DQ36" s="15"/>
+      <c r="DR36" s="15"/>
+      <c r="DS36" s="15"/>
+      <c r="DT36" s="15"/>
+      <c r="DU36" s="15"/>
+      <c r="DV36" s="15"/>
+      <c r="DW36" s="15"/>
+      <c r="DX36" s="15"/>
+      <c r="DY36" s="15"/>
+      <c r="DZ36" s="15"/>
+      <c r="EA36" s="15"/>
+      <c r="EB36" s="15"/>
+      <c r="EC36" s="15"/>
+      <c r="ED36" s="15"/>
+      <c r="EE36" s="15"/>
+      <c r="EF36" s="15"/>
+      <c r="EG36" s="15"/>
+      <c r="EH36" s="15"/>
+      <c r="EI36" s="15"/>
+      <c r="EJ36" s="15"/>
+      <c r="EK36" s="15"/>
+      <c r="EL36" s="15"/>
+      <c r="EM36" s="15"/>
+      <c r="EN36" s="15"/>
+      <c r="EO36" s="15"/>
+      <c r="EP36" s="15"/>
+      <c r="EQ36" s="15"/>
+      <c r="ER36" s="15"/>
+      <c r="ES36" s="15"/>
+      <c r="ET36" s="15"/>
+      <c r="EU36" s="15"/>
+      <c r="EV36" s="15"/>
+      <c r="EW36" s="15"/>
+      <c r="EX36" s="15"/>
+      <c r="EY36" s="15"/>
+      <c r="EZ36" s="15"/>
+      <c r="FA36" s="15"/>
+      <c r="FB36" s="15"/>
+      <c r="FC36" s="15"/>
+      <c r="FD36" s="15"/>
+      <c r="FE36" s="15"/>
+      <c r="FF36" s="15"/>
+      <c r="FG36" s="15"/>
+      <c r="FH36" s="15"/>
+      <c r="FI36" s="15"/>
+      <c r="FJ36" s="15"/>
+      <c r="FK36" s="15"/>
+      <c r="FL36" s="15"/>
+      <c r="FM36" s="15"/>
+      <c r="FN36" s="15"/>
+      <c r="FO36" s="15"/>
+      <c r="FP36" s="15"/>
+      <c r="FQ36" s="15"/>
+      <c r="FR36" s="15"/>
+      <c r="FS36" s="15"/>
+      <c r="FT36" s="15"/>
+      <c r="FU36" s="15"/>
+      <c r="FV36" s="15"/>
+      <c r="FW36" s="15"/>
+      <c r="FX36" s="15"/>
+      <c r="FY36" s="15"/>
+      <c r="FZ36" s="15"/>
+      <c r="GA36" s="15"/>
+      <c r="GB36" s="15"/>
+      <c r="GC36" s="15"/>
+      <c r="GD36" s="15"/>
+      <c r="GE36" s="15"/>
+      <c r="GF36" s="15"/>
+      <c r="GG36" s="15"/>
+      <c r="GH36" s="15"/>
+      <c r="GI36" s="15"/>
+      <c r="GJ36" s="15"/>
+      <c r="GK36" s="15"/>
+      <c r="GL36" s="15"/>
+      <c r="GM36" s="15"/>
+      <c r="GN36" s="15"/>
+      <c r="GO36" s="15"/>
+      <c r="GP36" s="15"/>
+      <c r="GQ36" s="15"/>
+      <c r="GR36" s="15"/>
+      <c r="GS36" s="15"/>
+      <c r="GT36" s="15"/>
+      <c r="GU36" s="15"/>
+      <c r="GV36" s="15"/>
+      <c r="GW36" s="15"/>
+      <c r="GX36" s="15"/>
+      <c r="GY36" s="15"/>
+      <c r="GZ36" s="15"/>
+      <c r="HA36" s="15"/>
+      <c r="HB36" s="15"/>
+      <c r="HC36" s="15"/>
+      <c r="HD36" s="15"/>
+      <c r="HE36" s="15"/>
+      <c r="HF36" s="15"/>
+      <c r="HG36" s="15"/>
+      <c r="HH36" s="15"/>
+      <c r="HI36" s="15"/>
+      <c r="HJ36" s="15"/>
+      <c r="HK36" s="15"/>
+      <c r="HL36" s="15"/>
+      <c r="HM36" s="15"/>
+      <c r="HN36" s="15"/>
+      <c r="HO36" s="15"/>
+      <c r="HP36" s="15"/>
+      <c r="HQ36" s="15"/>
+      <c r="HR36" s="15"/>
+      <c r="HS36" s="15"/>
+      <c r="HT36" s="15"/>
+      <c r="HU36" s="15"/>
+      <c r="HV36" s="15"/>
+      <c r="HW36" s="15"/>
+      <c r="HX36" s="15"/>
+      <c r="HY36" s="15"/>
+      <c r="HZ36" s="15"/>
+      <c r="IA36" s="15"/>
+      <c r="IB36" s="15"/>
+      <c r="IC36" s="15"/>
+      <c r="ID36" s="15"/>
+      <c r="IE36" s="15"/>
+      <c r="IF36" s="15"/>
+      <c r="IG36" s="15"/>
+      <c r="IH36" s="15"/>
+      <c r="II36" s="15"/>
+      <c r="IJ36" s="15"/>
+      <c r="IK36" s="15"/>
+      <c r="IL36" s="15"/>
+      <c r="IM36" s="15"/>
+      <c r="IN36" s="15"/>
+      <c r="IO36" s="15"/>
+      <c r="IP36" s="15"/>
+      <c r="IQ36" s="15"/>
+      <c r="IR36" s="15"/>
+      <c r="IS36" s="15"/>
+      <c r="IT36" s="15"/>
+      <c r="IU36" s="15"/>
+      <c r="IV36" s="15"/>
+      <c r="IW36" s="15"/>
+      <c r="IX36" s="15"/>
+      <c r="IY36" s="15"/>
+      <c r="IZ36" s="15"/>
+      <c r="JA36" s="15"/>
+      <c r="JB36" s="15"/>
+      <c r="JC36" s="15"/>
+      <c r="JD36" s="15"/>
+      <c r="JE36" s="15"/>
+      <c r="JF36" s="15"/>
+      <c r="JG36" s="15"/>
+      <c r="JH36" s="15"/>
+      <c r="JI36" s="15"/>
+      <c r="JJ36" s="15"/>
+      <c r="JK36" s="15"/>
+      <c r="JL36" s="15"/>
+      <c r="JM36" s="15"/>
+      <c r="JN36" s="15"/>
+      <c r="JO36" s="15"/>
+      <c r="JP36" s="15"/>
+      <c r="JQ36" s="15"/>
+      <c r="JR36" s="15"/>
+      <c r="JS36" s="15"/>
+      <c r="JT36" s="15"/>
+      <c r="JU36" s="15"/>
+      <c r="JV36" s="15"/>
+      <c r="JW36" s="15"/>
+      <c r="JX36" s="15"/>
+      <c r="JY36" s="15"/>
+      <c r="JZ36" s="15"/>
+      <c r="KA36" s="15"/>
+      <c r="KB36" s="15"/>
+      <c r="KC36" s="15"/>
+      <c r="KD36" s="15"/>
+      <c r="KE36" s="15"/>
+      <c r="KF36" s="15"/>
+      <c r="KG36" s="15"/>
+      <c r="KH36" s="15"/>
+      <c r="KI36" s="15"/>
+      <c r="KJ36" s="15"/>
+      <c r="KK36" s="15"/>
+      <c r="KL36" s="15"/>
+      <c r="KM36" s="15"/>
+      <c r="KN36" s="15"/>
+      <c r="KO36" s="15"/>
+      <c r="KP36" s="15"/>
+      <c r="KQ36" s="15"/>
+      <c r="KR36" s="15"/>
+      <c r="KS36" s="15"/>
+      <c r="KT36" s="15"/>
+      <c r="KU36" s="15"/>
+      <c r="KV36" s="15"/>
+      <c r="KW36" s="15"/>
+      <c r="KX36" s="15"/>
+      <c r="KY36" s="15"/>
+      <c r="KZ36" s="15"/>
+      <c r="LA36" s="15"/>
+      <c r="LB36" s="15"/>
+      <c r="LC36" s="15"/>
+      <c r="LD36" s="15"/>
+      <c r="LE36" s="15"/>
+      <c r="LF36" s="15"/>
+      <c r="LG36" s="15"/>
+      <c r="LH36" s="15"/>
+      <c r="LI36" s="15"/>
+      <c r="LJ36" s="15"/>
+      <c r="LK36" s="15"/>
+      <c r="LL36" s="15"/>
+      <c r="LM36" s="15"/>
+      <c r="LN36" s="15"/>
+      <c r="LO36" s="15"/>
+      <c r="LP36" s="15"/>
+      <c r="LQ36" s="15"/>
+      <c r="LR36" s="15"/>
+      <c r="LS36" s="15"/>
+      <c r="LT36" s="15"/>
+      <c r="LU36" s="15"/>
+      <c r="LV36" s="15"/>
+      <c r="LW36" s="15"/>
+      <c r="LX36" s="15"/>
+      <c r="LY36" s="15"/>
+      <c r="LZ36" s="15"/>
+      <c r="MA36" s="15"/>
+      <c r="MB36" s="15"/>
+      <c r="MC36" s="15"/>
+      <c r="MD36" s="15"/>
+      <c r="ME36" s="15"/>
+      <c r="MF36" s="15"/>
+      <c r="MG36" s="15"/>
+      <c r="MH36" s="15"/>
+      <c r="MI36" s="15"/>
+      <c r="MJ36" s="15"/>
+      <c r="MK36" s="15"/>
+      <c r="ML36" s="15"/>
+      <c r="MM36" s="15"/>
+      <c r="MN36" s="15"/>
+      <c r="MO36" s="15"/>
+      <c r="MP36" s="15"/>
+      <c r="MQ36" s="15"/>
+      <c r="MR36" s="15"/>
+      <c r="MS36" s="15"/>
+      <c r="MT36" s="15"/>
+      <c r="MU36" s="15"/>
+      <c r="MV36" s="15"/>
+      <c r="MW36" s="15"/>
+      <c r="MX36" s="15"/>
+      <c r="MY36" s="15"/>
+      <c r="MZ36" s="15"/>
+      <c r="NA36" s="15"/>
+      <c r="NB36" s="15"/>
+      <c r="NC36" s="15"/>
+      <c r="ND36" s="15"/>
+      <c r="NE36" s="15"/>
+      <c r="NF36" s="15"/>
+      <c r="NG36" s="15"/>
+      <c r="NH36" s="15"/>
+      <c r="NI36" s="15"/>
+      <c r="NJ36" s="15"/>
+      <c r="NK36" s="15"/>
+      <c r="NL36" s="15"/>
+      <c r="NM36" s="15"/>
+      <c r="NN36" s="15"/>
+      <c r="NO36" s="15"/>
+      <c r="NP36" s="15"/>
+      <c r="NQ36" s="15"/>
+      <c r="NR36" s="15"/>
+      <c r="NS36" s="15"/>
+      <c r="NT36" s="15"/>
+      <c r="NU36" s="15"/>
+      <c r="NV36" s="15"/>
+      <c r="NW36" s="15"/>
+      <c r="NX36" s="15"/>
+      <c r="NY36" s="15"/>
+      <c r="NZ36" s="15"/>
+      <c r="OA36" s="15"/>
+      <c r="OB36" s="15"/>
+      <c r="OC36" s="15"/>
+      <c r="OD36" s="15"/>
+      <c r="OE36" s="15"/>
+      <c r="OF36" s="15"/>
+      <c r="OG36" s="15"/>
+      <c r="OH36" s="15"/>
+      <c r="OI36" s="15"/>
+      <c r="OJ36" s="15"/>
+      <c r="OK36" s="15"/>
+      <c r="OL36" s="15"/>
+      <c r="OM36" s="15"/>
+      <c r="ON36" s="15"/>
+      <c r="OO36" s="15"/>
+      <c r="OP36" s="15"/>
+      <c r="OQ36" s="15"/>
+      <c r="OR36" s="15"/>
+      <c r="OS36" s="15"/>
+      <c r="OT36" s="15"/>
+      <c r="OU36" s="15"/>
+      <c r="OV36" s="15"/>
+      <c r="OW36" s="15"/>
+      <c r="OX36" s="15"/>
+      <c r="OY36" s="15"/>
+      <c r="OZ36" s="15"/>
+      <c r="PA36" s="15"/>
+      <c r="PB36" s="15"/>
+      <c r="PC36" s="15"/>
+      <c r="PD36" s="15"/>
+      <c r="PE36" s="15"/>
+      <c r="PF36" s="15"/>
+      <c r="PG36" s="15"/>
+      <c r="PH36" s="15"/>
+      <c r="PI36" s="15"/>
+      <c r="PJ36" s="15"/>
+      <c r="PK36" s="15"/>
+      <c r="PL36" s="15"/>
+      <c r="PM36" s="15"/>
+      <c r="PN36" s="15"/>
+      <c r="PO36" s="15"/>
+      <c r="PP36" s="15"/>
+      <c r="PQ36" s="15"/>
+      <c r="PR36" s="15"/>
+      <c r="PS36" s="15"/>
+      <c r="PT36" s="15"/>
+      <c r="PU36" s="15"/>
+      <c r="PV36" s="15"/>
+      <c r="PW36" s="15"/>
+      <c r="PX36" s="15"/>
+      <c r="PY36" s="15"/>
+      <c r="PZ36" s="15"/>
+      <c r="QA36" s="15"/>
+      <c r="QB36" s="15"/>
+      <c r="QC36" s="15"/>
+      <c r="QD36" s="15"/>
+      <c r="QE36" s="15"/>
+      <c r="QF36" s="15"/>
+      <c r="QG36" s="15"/>
+      <c r="QH36" s="15"/>
+      <c r="QI36" s="15"/>
+      <c r="QJ36" s="15"/>
+      <c r="QK36" s="15"/>
+      <c r="QL36" s="15"/>
+      <c r="QM36" s="15"/>
+      <c r="QN36" s="15"/>
+      <c r="QO36" s="15"/>
+      <c r="QP36" s="15"/>
+      <c r="QQ36" s="15"/>
+      <c r="QR36" s="15"/>
+      <c r="QS36" s="15"/>
+      <c r="QT36" s="15"/>
+      <c r="QU36" s="15"/>
+      <c r="QV36" s="15"/>
+      <c r="QW36" s="15"/>
+      <c r="QX36" s="15"/>
+      <c r="QY36" s="15"/>
+      <c r="QZ36" s="15"/>
+      <c r="RA36" s="15"/>
+      <c r="RB36" s="15"/>
+      <c r="RC36" s="15"/>
+      <c r="RD36" s="15"/>
+      <c r="RE36" s="15"/>
+      <c r="RF36" s="15"/>
+      <c r="RG36" s="15"/>
+      <c r="RH36" s="15"/>
+      <c r="RI36" s="15"/>
+      <c r="RJ36" s="15"/>
+      <c r="RK36" s="15"/>
+      <c r="RL36" s="15"/>
+      <c r="RM36" s="15"/>
+      <c r="RN36" s="15"/>
+      <c r="RO36" s="15"/>
+      <c r="RP36" s="15"/>
+      <c r="RQ36" s="15"/>
+      <c r="RR36" s="15"/>
+      <c r="RS36" s="15"/>
+      <c r="RT36" s="15"/>
+      <c r="RU36" s="15"/>
+      <c r="RV36" s="15"/>
+      <c r="RW36" s="15"/>
+      <c r="RX36" s="15"/>
+      <c r="RY36" s="15"/>
+      <c r="RZ36" s="15"/>
+      <c r="SA36" s="15"/>
+      <c r="SB36" s="15"/>
+      <c r="SC36" s="15"/>
+      <c r="SD36" s="15"/>
+      <c r="SE36" s="15"/>
+      <c r="SF36" s="15"/>
+      <c r="SG36" s="15"/>
+      <c r="SH36" s="15"/>
+      <c r="SI36" s="15"/>
+      <c r="SJ36" s="15"/>
+      <c r="SK36" s="15"/>
+      <c r="SL36" s="15"/>
+      <c r="SM36" s="15"/>
+      <c r="SN36" s="15"/>
+      <c r="SO36" s="15"/>
+      <c r="SP36" s="15"/>
+      <c r="SQ36" s="15"/>
+      <c r="SR36" s="15"/>
+      <c r="SS36" s="15"/>
+      <c r="ST36" s="15"/>
+      <c r="SU36" s="15"/>
+      <c r="SV36" s="15"/>
+      <c r="SW36" s="15"/>
+      <c r="SX36" s="15"/>
+      <c r="SY36" s="15"/>
+      <c r="SZ36" s="15"/>
+      <c r="TA36" s="15"/>
+      <c r="TB36" s="15"/>
+      <c r="TC36" s="15"/>
+      <c r="TD36" s="15"/>
+      <c r="TE36" s="15"/>
+      <c r="TF36" s="15"/>
+      <c r="TG36" s="15"/>
+      <c r="TH36" s="15"/>
+      <c r="TI36" s="15"/>
+      <c r="TJ36" s="15"/>
+      <c r="TK36" s="15"/>
+      <c r="TL36" s="15"/>
+      <c r="TM36" s="15"/>
+      <c r="TN36" s="15"/>
+      <c r="TO36" s="15"/>
+      <c r="TP36" s="15"/>
+      <c r="TQ36" s="15"/>
+      <c r="TR36" s="15"/>
+      <c r="TS36" s="15"/>
+      <c r="TT36" s="15"/>
+      <c r="TU36" s="15"/>
+      <c r="TV36" s="15"/>
+      <c r="TW36" s="15"/>
+      <c r="TX36" s="15"/>
+      <c r="TY36" s="15"/>
+      <c r="TZ36" s="15"/>
+      <c r="UA36" s="15"/>
+      <c r="UB36" s="15"/>
+      <c r="UC36" s="15"/>
+      <c r="UD36" s="15"/>
+      <c r="UE36" s="15"/>
+      <c r="UF36" s="15"/>
+      <c r="UG36" s="15"/>
+      <c r="UH36" s="15"/>
+      <c r="UI36" s="15"/>
+      <c r="UJ36" s="15"/>
+      <c r="UK36" s="15"/>
+      <c r="UL36" s="15"/>
+      <c r="UM36" s="15"/>
+      <c r="UN36" s="15"/>
+      <c r="UO36" s="15"/>
+      <c r="UP36" s="15"/>
+      <c r="UQ36" s="15"/>
+      <c r="UR36" s="15"/>
+      <c r="US36" s="15"/>
+      <c r="UT36" s="15"/>
+      <c r="UU36" s="15"/>
+      <c r="UV36" s="15"/>
+      <c r="UW36" s="15"/>
+      <c r="UX36" s="15"/>
+      <c r="UY36" s="15"/>
+      <c r="UZ36" s="15"/>
+      <c r="VA36" s="15"/>
+      <c r="VB36" s="15"/>
+      <c r="VC36" s="15"/>
+      <c r="VD36" s="15"/>
+      <c r="VE36" s="15"/>
+      <c r="VF36" s="15"/>
+      <c r="VG36" s="15"/>
+      <c r="VH36" s="15"/>
+      <c r="VI36" s="15"/>
+      <c r="VJ36" s="15"/>
+      <c r="VK36" s="15"/>
+      <c r="VL36" s="15"/>
+      <c r="VM36" s="15"/>
+      <c r="VN36" s="15"/>
+      <c r="VO36" s="15"/>
+      <c r="VP36" s="15"/>
+      <c r="VQ36" s="15"/>
+      <c r="VR36" s="15"/>
+      <c r="VS36" s="15"/>
+      <c r="VT36" s="15"/>
+      <c r="VU36" s="15"/>
+      <c r="VV36" s="15"/>
+      <c r="VW36" s="15"/>
+      <c r="VX36" s="15"/>
+      <c r="VY36" s="15"/>
+      <c r="VZ36" s="15"/>
+      <c r="WA36" s="15"/>
+      <c r="WB36" s="15"/>
+      <c r="WC36" s="15"/>
+      <c r="WD36" s="15"/>
+      <c r="WE36" s="15"/>
+      <c r="WF36" s="15"/>
+      <c r="WG36" s="15"/>
+      <c r="WH36" s="15"/>
+      <c r="WI36" s="15"/>
+      <c r="WJ36" s="15"/>
+      <c r="WK36" s="15"/>
+      <c r="WL36" s="15"/>
+      <c r="WM36" s="15"/>
+      <c r="WN36" s="15"/>
+      <c r="WO36" s="15"/>
+      <c r="WP36" s="15"/>
+      <c r="WQ36" s="15"/>
+      <c r="WR36" s="15"/>
+      <c r="WS36" s="15"/>
+      <c r="WT36" s="15"/>
+      <c r="WU36" s="15"/>
+      <c r="WV36" s="15"/>
+      <c r="WW36" s="15"/>
+      <c r="WX36" s="15"/>
+      <c r="WY36" s="15"/>
+      <c r="WZ36" s="15"/>
+      <c r="XA36" s="15"/>
+      <c r="XB36" s="15"/>
+      <c r="XC36" s="15"/>
+      <c r="XD36" s="15"/>
+      <c r="XE36" s="15"/>
+      <c r="XF36" s="15"/>
+      <c r="XG36" s="15"/>
+      <c r="XH36" s="15"/>
+      <c r="XI36" s="15"/>
+      <c r="XJ36" s="15"/>
+      <c r="XK36" s="15"/>
+      <c r="XL36" s="15"/>
+      <c r="XM36" s="15"/>
+      <c r="XN36" s="15"/>
+      <c r="XO36" s="15"/>
+      <c r="XP36" s="15"/>
+      <c r="XQ36" s="15"/>
+      <c r="XR36" s="15"/>
+      <c r="XS36" s="15"/>
+      <c r="XT36" s="15"/>
+      <c r="XU36" s="15"/>
+      <c r="XV36" s="15"/>
+      <c r="XW36" s="15"/>
+      <c r="XX36" s="15"/>
+      <c r="XY36" s="15"/>
+      <c r="XZ36" s="15"/>
+      <c r="YA36" s="15"/>
+      <c r="YB36" s="15"/>
+      <c r="YC36" s="15"/>
+      <c r="YD36" s="15"/>
+      <c r="YE36" s="15"/>
+      <c r="YF36" s="15"/>
+      <c r="YG36" s="15"/>
+      <c r="YH36" s="15"/>
+      <c r="YI36" s="15"/>
+      <c r="YJ36" s="15"/>
+      <c r="YK36" s="15"/>
+      <c r="YL36" s="15"/>
+      <c r="YM36" s="15"/>
+      <c r="YN36" s="15"/>
+      <c r="YO36" s="15"/>
+      <c r="YP36" s="15"/>
+      <c r="YQ36" s="15"/>
+      <c r="YR36" s="15"/>
+      <c r="YS36" s="15"/>
+      <c r="YT36" s="15"/>
+      <c r="YU36" s="15"/>
+      <c r="YV36" s="15"/>
+      <c r="YW36" s="15"/>
+      <c r="YX36" s="15"/>
+      <c r="YY36" s="15"/>
+      <c r="YZ36" s="15"/>
+      <c r="ZA36" s="15"/>
+      <c r="ZB36" s="15"/>
+      <c r="ZC36" s="15"/>
+      <c r="ZD36" s="15"/>
+      <c r="ZE36" s="15"/>
+      <c r="ZF36" s="15"/>
+      <c r="ZG36" s="15"/>
+      <c r="ZH36" s="15"/>
+      <c r="ZI36" s="15"/>
+      <c r="ZJ36" s="15"/>
+      <c r="ZK36" s="15"/>
+      <c r="ZL36" s="15"/>
+      <c r="ZM36" s="15"/>
+      <c r="ZN36" s="15"/>
+      <c r="ZO36" s="15"/>
+      <c r="ZP36" s="15"/>
+      <c r="ZQ36" s="15"/>
+      <c r="ZR36" s="15"/>
+      <c r="ZS36" s="15"/>
+      <c r="ZT36" s="15"/>
+      <c r="ZU36" s="15"/>
+      <c r="ZV36" s="15"/>
+      <c r="ZW36" s="15"/>
+      <c r="ZX36" s="15"/>
+      <c r="ZY36" s="15"/>
+      <c r="ZZ36" s="15"/>
+      <c r="AAA36" s="15"/>
+      <c r="AAB36" s="15"/>
+      <c r="AAC36" s="15"/>
+      <c r="AAD36" s="15"/>
+      <c r="AAE36" s="15"/>
+      <c r="AAF36" s="15"/>
+      <c r="AAG36" s="15"/>
+      <c r="AAH36" s="15"/>
+      <c r="AAI36" s="15"/>
+      <c r="AAJ36" s="15"/>
+      <c r="AAK36" s="15"/>
+      <c r="AAL36" s="15"/>
+      <c r="AAM36" s="15"/>
+      <c r="AAN36" s="15"/>
+      <c r="AAO36" s="15"/>
+      <c r="AAP36" s="15"/>
+      <c r="AAQ36" s="15"/>
+      <c r="AAR36" s="15"/>
+      <c r="AAS36" s="15"/>
+      <c r="AAT36" s="15"/>
+      <c r="AAU36" s="15"/>
+      <c r="AAV36" s="15"/>
+      <c r="AAW36" s="15"/>
+      <c r="AAX36" s="15"/>
+      <c r="AAY36" s="15"/>
+      <c r="AAZ36" s="15"/>
+      <c r="ABA36" s="15"/>
+      <c r="ABB36" s="15"/>
+      <c r="ABC36" s="15"/>
+      <c r="ABD36" s="15"/>
+      <c r="ABE36" s="15"/>
+      <c r="ABF36" s="15"/>
+      <c r="ABG36" s="15"/>
+      <c r="ABH36" s="15"/>
+      <c r="ABI36" s="15"/>
+      <c r="ABJ36" s="15"/>
+      <c r="ABK36" s="15"/>
+      <c r="ABL36" s="15"/>
+      <c r="ABM36" s="15"/>
+      <c r="ABN36" s="15"/>
+      <c r="ABO36" s="15"/>
+      <c r="ABP36" s="15"/>
+      <c r="ABQ36" s="15"/>
+      <c r="ABR36" s="15"/>
+      <c r="ABS36" s="15"/>
+      <c r="ABT36" s="15"/>
+      <c r="ABU36" s="15"/>
+      <c r="ABV36" s="15"/>
+      <c r="ABW36" s="15"/>
+      <c r="ABX36" s="15"/>
+      <c r="ABY36" s="15"/>
+      <c r="ABZ36" s="15"/>
+      <c r="ACA36" s="15"/>
+      <c r="ACB36" s="15"/>
+      <c r="ACC36" s="15"/>
+      <c r="ACD36" s="15"/>
+      <c r="ACE36" s="15"/>
+      <c r="ACF36" s="15"/>
+      <c r="ACG36" s="15"/>
+      <c r="ACH36" s="15"/>
+      <c r="ACI36" s="15"/>
+      <c r="ACJ36" s="15"/>
+      <c r="ACK36" s="15"/>
+      <c r="ACL36" s="15"/>
+      <c r="ACM36" s="15"/>
+      <c r="ACN36" s="15"/>
+      <c r="ACO36" s="15"/>
+      <c r="ACP36" s="15"/>
+      <c r="ACQ36" s="15"/>
+      <c r="ACR36" s="15"/>
+      <c r="ACS36" s="15"/>
+      <c r="ACT36" s="15"/>
+      <c r="ACU36" s="15"/>
+      <c r="ACV36" s="15"/>
+      <c r="ACW36" s="15"/>
+      <c r="ACX36" s="15"/>
+      <c r="ACY36" s="15"/>
+      <c r="ACZ36" s="15"/>
+      <c r="ADA36" s="15"/>
+      <c r="ADB36" s="15"/>
+      <c r="ADC36" s="15"/>
+      <c r="ADD36" s="15"/>
+      <c r="ADE36" s="15"/>
+      <c r="ADF36" s="15"/>
+      <c r="ADG36" s="15"/>
+      <c r="ADH36" s="15"/>
+      <c r="ADI36" s="15"/>
+      <c r="ADJ36" s="15"/>
+      <c r="ADK36" s="15"/>
+      <c r="ADL36" s="15"/>
+      <c r="ADM36" s="15"/>
+      <c r="ADN36" s="15"/>
+      <c r="ADO36" s="15"/>
+      <c r="ADP36" s="15"/>
+      <c r="ADQ36" s="15"/>
+      <c r="ADR36" s="15"/>
+      <c r="ADS36" s="15"/>
+      <c r="ADT36" s="15"/>
+      <c r="ADU36" s="15"/>
+      <c r="ADV36" s="15"/>
+      <c r="ADW36" s="15"/>
+      <c r="ADX36" s="15"/>
+      <c r="ADY36" s="15"/>
+      <c r="ADZ36" s="15"/>
+      <c r="AEA36" s="15"/>
+      <c r="AEB36" s="15"/>
+      <c r="AEC36" s="15"/>
+      <c r="AED36" s="15"/>
+      <c r="AEE36" s="15"/>
+      <c r="AEF36" s="15"/>
+      <c r="AEG36" s="15"/>
+      <c r="AEH36" s="15"/>
+      <c r="AEI36" s="15"/>
+      <c r="AEJ36" s="15"/>
+      <c r="AEK36" s="15"/>
+      <c r="AEL36" s="15"/>
+      <c r="AEM36" s="15"/>
+      <c r="AEN36" s="15"/>
+      <c r="AEO36" s="15"/>
+      <c r="AEP36" s="15"/>
+      <c r="AEQ36" s="15"/>
+      <c r="AER36" s="15"/>
+      <c r="AES36" s="15"/>
+      <c r="AET36" s="15"/>
+      <c r="AEU36" s="15"/>
+      <c r="AEV36" s="15"/>
+      <c r="AEW36" s="15"/>
+      <c r="AEX36" s="15"/>
+      <c r="AEY36" s="15"/>
+      <c r="AEZ36" s="15"/>
+      <c r="AFA36" s="15"/>
+      <c r="AFB36" s="15"/>
+      <c r="AFC36" s="15"/>
+      <c r="AFD36" s="15"/>
+      <c r="AFE36" s="15"/>
+      <c r="AFF36" s="15"/>
+      <c r="AFG36" s="15"/>
+      <c r="AFH36" s="15"/>
+      <c r="AFI36" s="15"/>
+      <c r="AFJ36" s="15"/>
+      <c r="AFK36" s="15"/>
+      <c r="AFL36" s="15"/>
+      <c r="AFM36" s="15"/>
+      <c r="AFN36" s="15"/>
+      <c r="AFO36" s="15"/>
+      <c r="AFP36" s="15"/>
+      <c r="AFQ36" s="15"/>
+      <c r="AFR36" s="15"/>
+      <c r="AFS36" s="15"/>
+      <c r="AFT36" s="15"/>
+      <c r="AFU36" s="15"/>
+      <c r="AFV36" s="15"/>
+      <c r="AFW36" s="15"/>
+      <c r="AFX36" s="15"/>
+      <c r="AFY36" s="15"/>
+      <c r="AFZ36" s="15"/>
+      <c r="AGA36" s="15"/>
+      <c r="AGB36" s="15"/>
+      <c r="AGC36" s="15"/>
+      <c r="AGD36" s="15"/>
+      <c r="AGE36" s="15"/>
+      <c r="AGF36" s="15"/>
+      <c r="AGG36" s="15"/>
+      <c r="AGH36" s="15"/>
+      <c r="AGI36" s="15"/>
+      <c r="AGJ36" s="15"/>
+      <c r="AGK36" s="15"/>
+      <c r="AGL36" s="15"/>
+      <c r="AGM36" s="15"/>
+      <c r="AGN36" s="15"/>
+      <c r="AGO36" s="15"/>
+      <c r="AGP36" s="15"/>
+      <c r="AGQ36" s="15"/>
+      <c r="AGR36" s="15"/>
+      <c r="AGS36" s="15"/>
+      <c r="AGT36" s="15"/>
+      <c r="AGU36" s="15"/>
+      <c r="AGV36" s="15"/>
+      <c r="AGW36" s="15"/>
+      <c r="AGX36" s="15"/>
+      <c r="AGY36" s="15"/>
+      <c r="AGZ36" s="15"/>
+      <c r="AHA36" s="15"/>
+      <c r="AHB36" s="15"/>
+      <c r="AHC36" s="15"/>
+      <c r="AHD36" s="15"/>
+      <c r="AHE36" s="15"/>
+      <c r="AHF36" s="15"/>
+      <c r="AHG36" s="15"/>
+      <c r="AHH36" s="15"/>
+      <c r="AHI36" s="15"/>
+      <c r="AHJ36" s="15"/>
+      <c r="AHK36" s="15"/>
+      <c r="AHL36" s="15"/>
+      <c r="AHM36" s="15"/>
+      <c r="AHN36" s="15"/>
+      <c r="AHO36" s="15"/>
+      <c r="AHP36" s="15"/>
+      <c r="AHQ36" s="15"/>
+      <c r="AHR36" s="15"/>
+      <c r="AHS36" s="15"/>
+      <c r="AHT36" s="15"/>
+      <c r="AHU36" s="15"/>
+      <c r="AHV36" s="15"/>
+      <c r="AHW36" s="15"/>
+      <c r="AHX36" s="15"/>
+      <c r="AHY36" s="15"/>
+      <c r="AHZ36" s="15"/>
+      <c r="AIA36" s="15"/>
+      <c r="AIB36" s="15"/>
+      <c r="AIC36" s="15"/>
+      <c r="AID36" s="15"/>
+      <c r="AIE36" s="15"/>
+      <c r="AIF36" s="15"/>
+      <c r="AIG36" s="15"/>
+      <c r="AIH36" s="15"/>
+      <c r="AII36" s="15"/>
+      <c r="AIJ36" s="15"/>
+      <c r="AIK36" s="15"/>
+      <c r="AIL36" s="15"/>
+      <c r="AIM36" s="15"/>
+      <c r="AIN36" s="15"/>
+      <c r="AIO36" s="15"/>
+      <c r="AIP36" s="15"/>
+      <c r="AIQ36" s="15"/>
+      <c r="AIR36" s="15"/>
+      <c r="AIS36" s="15"/>
+      <c r="AIT36" s="15"/>
+      <c r="AIU36" s="15"/>
+      <c r="AIV36" s="15"/>
+      <c r="AIW36" s="15"/>
+      <c r="AIX36" s="15"/>
+      <c r="AIY36" s="15"/>
+      <c r="AIZ36" s="15"/>
+      <c r="AJA36" s="15"/>
+      <c r="AJB36" s="15"/>
+      <c r="AJC36" s="15"/>
+      <c r="AJD36" s="15"/>
+      <c r="AJE36" s="15"/>
+      <c r="AJF36" s="15"/>
+      <c r="AJG36" s="15"/>
+      <c r="AJH36" s="15"/>
+      <c r="AJI36" s="15"/>
+      <c r="AJJ36" s="15"/>
+      <c r="AJK36" s="15"/>
+      <c r="AJL36" s="15"/>
+      <c r="AJM36" s="15"/>
+      <c r="AJN36" s="15"/>
+      <c r="AJO36" s="15"/>
+      <c r="AJP36" s="15"/>
+      <c r="AJQ36" s="15"/>
+      <c r="AJR36" s="15"/>
+      <c r="AJS36" s="15"/>
+      <c r="AJT36" s="15"/>
+      <c r="AJU36" s="15"/>
+      <c r="AJV36" s="15"/>
+      <c r="AJW36" s="15"/>
+      <c r="AJX36" s="15"/>
+      <c r="AJY36" s="15"/>
+      <c r="AJZ36" s="15"/>
+      <c r="AKA36" s="15"/>
+      <c r="AKB36" s="15"/>
+      <c r="AKC36" s="15"/>
+      <c r="AKD36" s="15"/>
+      <c r="AKE36" s="15"/>
+      <c r="AKF36" s="15"/>
+      <c r="AKG36" s="15"/>
+      <c r="AKH36" s="15"/>
+      <c r="AKI36" s="15"/>
+      <c r="AKJ36" s="15"/>
+      <c r="AKK36" s="15"/>
+      <c r="AKL36" s="15"/>
+      <c r="AKM36" s="15"/>
+      <c r="AKN36" s="15"/>
+      <c r="AKO36" s="15"/>
+      <c r="AKP36" s="15"/>
+      <c r="AKQ36" s="15"/>
+      <c r="AKR36" s="15"/>
+      <c r="AKS36" s="15"/>
+      <c r="AKT36" s="15"/>
+      <c r="AKU36" s="15"/>
+      <c r="AKV36" s="15"/>
+      <c r="AKW36" s="15"/>
+      <c r="AKX36" s="15"/>
+      <c r="AKY36" s="15"/>
+      <c r="AKZ36" s="15"/>
+      <c r="ALA36" s="15"/>
+      <c r="ALB36" s="15"/>
+      <c r="ALC36" s="15"/>
+      <c r="ALD36" s="15"/>
+      <c r="ALE36" s="15"/>
+      <c r="ALF36" s="15"/>
+      <c r="ALG36" s="15"/>
+      <c r="ALH36" s="15"/>
+      <c r="ALI36" s="15"/>
+      <c r="ALJ36" s="15"/>
+      <c r="ALK36" s="15"/>
+      <c r="ALL36" s="15"/>
+      <c r="ALM36" s="15"/>
+      <c r="ALN36" s="15"/>
+      <c r="ALO36" s="15"/>
+      <c r="ALP36" s="15"/>
+      <c r="ALQ36" s="15"/>
+      <c r="ALR36" s="15"/>
+      <c r="ALS36" s="15"/>
+      <c r="ALT36" s="15"/>
+      <c r="ALU36" s="15"/>
+      <c r="ALV36" s="15"/>
+      <c r="ALW36" s="15"/>
+      <c r="ALX36" s="15"/>
+      <c r="ALY36" s="15"/>
+      <c r="ALZ36" s="15"/>
+      <c r="AMA36" s="15"/>
+      <c r="AMB36" s="15"/>
+      <c r="AMC36" s="15"/>
+      <c r="AMD36" s="15"/>
+      <c r="AME36" s="15"/>
+      <c r="AMF36" s="15"/>
+      <c r="AMG36" s="15"/>
+      <c r="AMH36" s="15"/>
+      <c r="AMI36" s="15"/>
+      <c r="AMJ36" s="15"/>
+      <c r="AMK36" s="15"/>
+      <c r="AML36" s="15"/>
+      <c r="AMM36" s="15"/>
+      <c r="AMN36" s="15"/>
     </row>
     <row r="37" spans="1:1028" ht="240" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">

</xml_diff>